<commit_message>
Update Oracle - wholesale minimal standard scenario.xlsx
</commit_message>
<xml_diff>
--- a/source/databricks/calculation_engine/tests/features/given_a_wholesale_calculation/when_minimal_standard_scenario/Oracle - wholesale minimal standard scenario.xlsx
+++ b/source/databricks/calculation_engine/tests/features/given_a_wholesale_calculation/when_minimal_standard_scenario/Oracle - wholesale minimal standard scenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\opengeh-wholesale\source\databricks\calculation_engine\tests\features\given_a_wholesale_calculation\when_minimal_standard_scenario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C5922D-E845-4567-93A7-FB10A6BADEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB31EB3E-37E5-4FFB-A553-56A8B89A7846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B26405EC-4681-4CC9-BF80-F87B3459AD72}"/>
+    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{B26405EC-4681-4CC9-BF80-F87B3459AD72}"/>
   </bookViews>
   <sheets>
     <sheet name="Hour1" sheetId="11" r:id="rId1"/>
@@ -362,9 +362,6 @@
     <t>Number</t>
   </si>
   <si>
-    <t>from_grid_area</t>
-  </si>
-  <si>
     <t>ga_brp_es</t>
   </si>
   <si>
@@ -470,7 +467,10 @@
     <t>170000000000000102</t>
   </si>
   <si>
-    <t>production</t>
+    <t>neighbor_grid_area_code</t>
+  </si>
+  <si>
+    <t>nonprofiled_consumption</t>
   </si>
 </sst>
 </file>
@@ -1422,53 +1422,54 @@
   </sheetPr>
   <dimension ref="A1:CN400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66:H68"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I84" sqref="I84:I87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.140625" style="1" customWidth="1"/>
-    <col min="16" max="17" width="11.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="32.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="1.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="40" width="8.7109375" style="1" customWidth="1"/>
-    <col min="41" max="16384" width="8.7109375" style="1"/>
+    <col min="14" max="14" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.1796875" style="1" customWidth="1"/>
+    <col min="16" max="17" width="11.7265625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="2.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="1.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="27.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="40" width="8.7265625" style="1" customWidth="1"/>
+    <col min="41" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:92" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:92" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="18" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>7</v>
@@ -1492,7 +1493,7 @@
         <v>75</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K1" s="14" t="s">
         <v>8</v>
@@ -1539,7 +1540,7 @@
         <v>17</v>
       </c>
       <c r="AG1" s="30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AH1" s="47" t="s">
         <v>81</v>
@@ -1548,7 +1549,7 @@
       <c r="AJ1" s="47"/>
       <c r="AK1" s="47"/>
     </row>
-    <row r="2" spans="1:92" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:92" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="18" t="s">
         <v>25</v>
       </c>
@@ -1556,13 +1557,13 @@
         <v>121</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -1573,19 +1574,19 @@
         <v>0</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L2" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="N2" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="O2" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>92</v>
       </c>
       <c r="P2" s="29"/>
       <c r="Q2" s="29"/>
@@ -1622,35 +1623,35 @@
         <v>800</v>
       </c>
       <c r="AE2" s="27" t="str" cm="1">
-        <f t="array" ref="AE2:AE3">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn._xlws.FILTER(AE28:AE41,AE28:AE41 &lt;&gt; "")))</f>
-        <v>2000000000000</v>
+        <f t="array" ref="AE2">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn._xlws.FILTER(AE28:AE41,AE28:AE41 &lt;&gt; "")))</f>
+        <v>3000000000000</v>
       </c>
       <c r="AF2" s="27" t="str" cm="1">
-        <f t="array" ref="AF2:AF3">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn._xlws.FILTER(AF28:AF40,AF28:AF40 &lt;&gt; "")))</f>
-        <v>2200000000000</v>
+        <f t="array" ref="AF2">_xlfn._xlws.SORT(_xlfn.UNIQUE(_xlfn._xlws.FILTER(AF28:AF40,AF28:AF40 &lt;&gt; "")))</f>
+        <v>3300000000000</v>
       </c>
       <c r="AG2" s="27" t="str">
         <f>IF(B$2="production","E18",IF($B$2="flex_consumption","D01","E02"))</f>
-        <v>E18</v>
+        <v>E02</v>
       </c>
       <c r="AH2" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI2" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="AI2" s="24" t="s">
+      <c r="AJ2" s="27" t="s">
         <v>109</v>
-      </c>
-      <c r="AJ2" s="27" t="s">
-        <v>110</v>
       </c>
       <c r="AK2" s="2"/>
       <c r="AL2" s="2"/>
     </row>
-    <row r="3" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C3" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="12"/>
@@ -1662,19 +1663,19 @@
         <v>0</v>
       </c>
       <c r="K3" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="M3" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="L3" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>99</v>
-      </c>
       <c r="N3" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P3" s="29"/>
       <c r="Q3" s="29"/>
@@ -1709,12 +1710,8 @@
       <c r="AD3" s="24" t="str">
         <v>801</v>
       </c>
-      <c r="AE3" s="24" t="str">
-        <v>4000000000000</v>
-      </c>
-      <c r="AF3" s="24" t="str">
-        <v>4400000000000</v>
-      </c>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
       <c r="AG3" s="24"/>
       <c r="AH3" s="27" t="str" cm="1">
         <f t="array" ref="AH3">_xlfn.UNIQUE(_xlfn._xlws.FILTER(_xlfn.VSTACK(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(TableDay1[from_ga],(TableDay1[from_ga]=$AD$2)+(TableDay1[to_ga]=$AD$2)),_xlfn._xlws.FILTER(TableDay1[from_ga],(TableDay1[from_ga]=$AD$2)+(TableDay1[to_ga]=$AD$2))&lt;&gt;AD2),IFERROR(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(TableDay1[to_ga],(TableDay1[from_ga]=$AD$2)+(TableDay1[to_ga]=$AD$2)),_xlfn._xlws.FILTER(TableDay1[to_ga],(TableDay1[from_ga]=$AD$2)+(TableDay1[to_ga]=$AD$2))&lt;&gt;AD2),""),IFERROR(IF(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(TableDay1[ga_id],TableDay1[from_ga]=TableDay1[to_ga]),_xlfn._xlws.FILTER(TableDay1[ga_id],TableDay1[from_ga]=TableDay1[to_ga])&lt;&gt;AD2),_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(TableDay1[ga_id],TableDay1[from_ga]=TableDay1[to_ga]),_xlfn._xlws.FILTER(TableDay1[ga_id],TableDay1[from_ga]=TableDay1[to_ga])&lt;&gt;AD2)&lt;&gt;0)&gt;0,AD2,""),"")),_xlfn.VSTACK(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(TableDay1[from_ga],(TableDay1[from_ga]=$AD$2)+(TableDay1[to_ga]=$AD$2)),_xlfn._xlws.FILTER(TableDay1[from_ga],(TableDay1[from_ga]=$AD$2)+(TableDay1[to_ga]=$AD$2))&lt;&gt;AD2),IFERROR(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(TableDay1[to_ga],(TableDay1[from_ga]=$AD$2)+(TableDay1[to_ga]=$AD$2)),_xlfn._xlws.FILTER(TableDay1[to_ga],(TableDay1[from_ga]=$AD$2)+(TableDay1[to_ga]=$AD$2))&lt;&gt;AD2),""),IFERROR(IF(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(TableDay1[ga_id],TableDay1[from_ga]=TableDay1[to_ga]),_xlfn._xlws.FILTER(TableDay1[ga_id],TableDay1[from_ga]=TableDay1[to_ga])&lt;&gt;AD2),_xlfn._xlws.FILTER(_xlfn._xlws.FILTER(TableDay1[ga_id],TableDay1[from_ga]=TableDay1[to_ga]),_xlfn._xlws.FILTER(TableDay1[ga_id],TableDay1[from_ga]=TableDay1[to_ga])&lt;&gt;AD2)&lt;&gt;0)&gt;0,AD2,""),""))&lt;&gt;""))</f>
@@ -1738,15 +1735,15 @@
       <c r="AP3" s="24"/>
       <c r="AQ3" s="24"/>
     </row>
-    <row r="4" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C4" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -1757,17 +1754,17 @@
         <v>0</v>
       </c>
       <c r="K4" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="M4" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>91</v>
       </c>
       <c r="N4" s="10"/>
       <c r="O4" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P4" s="29"/>
       <c r="Q4" s="29"/>
@@ -1818,7 +1815,7 @@
       <c r="AP4" s="24"/>
       <c r="AQ4" s="24"/>
     </row>
-    <row r="5" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="11"/>
@@ -1835,7 +1832,7 @@
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P5" s="29"/>
       <c r="Q5" s="29"/>
@@ -1886,15 +1883,15 @@
       <c r="AP5" s="24"/>
       <c r="AQ5" s="24"/>
     </row>
-    <row r="6" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C6" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F6" s="12">
         <v>20</v>
@@ -1907,17 +1904,17 @@
         <v>20</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N6" s="10"/>
       <c r="O6" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P6" s="29"/>
       <c r="Q6" s="29"/>
@@ -1951,15 +1948,15 @@
       <c r="AP6" s="24"/>
       <c r="AQ6" s="24"/>
     </row>
-    <row r="7" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C7" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F7" s="12">
         <v>2.5</v>
@@ -1978,17 +1975,17 @@
         <v>17.5</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N7" s="10"/>
       <c r="O7" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P7" s="29"/>
       <c r="Q7" s="29"/>
@@ -2022,12 +2019,12 @@
       <c r="AP7" s="24"/>
       <c r="AQ7" s="24"/>
     </row>
-    <row r="8" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C8" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="12">
@@ -2041,17 +2038,17 @@
         <v>40.158999999999999</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N8" s="10"/>
       <c r="O8" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P8" s="29"/>
       <c r="Q8" s="29"/>
@@ -2085,7 +2082,7 @@
       <c r="AP8" s="24"/>
       <c r="AQ8" s="24"/>
     </row>
-    <row r="9" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="11"/>
@@ -2102,7 +2099,7 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P9" s="29"/>
       <c r="Q9" s="29"/>
@@ -2148,12 +2145,12 @@
       <c r="AP9" s="24"/>
       <c r="AQ9" s="24"/>
     </row>
-    <row r="10" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C10" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="12"/>
@@ -2165,17 +2162,17 @@
         <v>0</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P10" s="29"/>
       <c r="Q10" s="29"/>
@@ -2188,24 +2185,24 @@
       </c>
       <c r="T10" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[brp_id],MATCH(U10,TableDay1[es_id],0)),"")</f>
-        <v>2200000000000</v>
+        <v>3300000000000</v>
       </c>
       <c r="U10" s="26" t="str">
         <f>IF(AE$2=0,"",AE$2)</f>
-        <v>2000000000000</v>
+        <v>3000000000000</v>
       </c>
       <c r="V10" s="20">
         <f>SUMIFS(TableDay1[TotalHour],TableDay1[es_id],U10,IF(B$2="production",TableDay1[type],TableDay1[settlement_method]),AG$2,TableDay1[resolution],"PT1H")/4</f>
-        <v>10.03975</v>
+        <v>5</v>
       </c>
       <c r="W10" s="19">
         <f>V10</f>
-        <v>10.03975</v>
+        <v>5</v>
       </c>
       <c r="X10" s="19"/>
       <c r="Y10" s="23">
         <f t="shared" ref="Y10:Y33" si="1">ROUND(W10, 3)</f>
-        <v>10.039999999999999</v>
+        <v>5</v>
       </c>
       <c r="Z10" s="27"/>
       <c r="AA10" s="24"/>
@@ -2229,12 +2226,12 @@
       <c r="AP10" s="24"/>
       <c r="AQ10" s="24"/>
     </row>
-    <row r="11" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C11" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="12">
@@ -2248,19 +2245,19 @@
         <v>3.3570000000000002</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P11" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q11" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R11" s="15" t="s">
         <v>73</v>
@@ -2271,27 +2268,27 @@
       </c>
       <c r="T11" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[brp_id],MATCH(U11,TableDay1[es_id],0)),"")</f>
-        <v>2200000000000</v>
+        <v>3300000000000</v>
       </c>
       <c r="U11" s="26" t="str">
         <f t="shared" ref="U11:V13" si="2">U$10</f>
-        <v>2000000000000</v>
+        <v>3000000000000</v>
       </c>
       <c r="V11" s="19">
         <f t="shared" si="2"/>
-        <v>10.03975</v>
+        <v>5</v>
       </c>
       <c r="W11" s="19">
         <f>X11+W10</f>
-        <v>10.0395</v>
+        <v>5</v>
       </c>
       <c r="X11" s="19">
         <f>V11-Y10</f>
-        <v>-2.4999999999941735E-4</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="23">
         <f t="shared" si="1"/>
-        <v>10.039999999999999</v>
+        <v>5</v>
       </c>
       <c r="Z11" s="27"/>
       <c r="AA11" s="24"/>
@@ -2315,7 +2312,7 @@
       <c r="AP11" s="24"/>
       <c r="AQ11" s="24"/>
     </row>
-    <row r="12" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="11"/>
@@ -2343,37 +2340,37 @@
       </c>
       <c r="T12" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[brp_id],MATCH(U12,TableDay1[es_id],0)),"")</f>
-        <v>2200000000000</v>
+        <v>3300000000000</v>
       </c>
       <c r="U12" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>2000000000000</v>
+        <v>3000000000000</v>
       </c>
       <c r="V12" s="19">
         <f t="shared" si="2"/>
-        <v>10.03975</v>
+        <v>5</v>
       </c>
       <c r="W12" s="19">
         <f>X12+W11</f>
-        <v>10.039250000000001</v>
+        <v>5</v>
       </c>
       <c r="X12" s="19">
         <f>V12-Y11</f>
-        <v>-2.4999999999941735E-4</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="23">
         <f t="shared" si="1"/>
-        <v>10.039</v>
+        <v>5</v>
       </c>
       <c r="Z12" s="27"/>
       <c r="AA12" s="24"/>
       <c r="AC12" s="27"/>
       <c r="AD12" s="36"/>
       <c r="AE12" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF12" s="36" t="s">
         <v>101</v>
-      </c>
-      <c r="AF12" s="36" t="s">
-        <v>102</v>
       </c>
       <c r="AG12" s="36"/>
       <c r="AH12" s="35"/>
@@ -2391,7 +2388,7 @@
       <c r="AP12" s="24"/>
       <c r="AQ12" s="24"/>
     </row>
-    <row r="13" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="11"/>
@@ -2419,27 +2416,27 @@
       </c>
       <c r="T13" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[brp_id],MATCH(U13,TableDay1[es_id],0)),"")</f>
-        <v>2200000000000</v>
+        <v>3300000000000</v>
       </c>
       <c r="U13" s="26" t="str">
         <f t="shared" si="2"/>
-        <v>2000000000000</v>
+        <v>3000000000000</v>
       </c>
       <c r="V13" s="19">
         <f t="shared" si="2"/>
-        <v>10.03975</v>
+        <v>5</v>
       </c>
       <c r="W13" s="19">
         <f>X13+W12</f>
-        <v>10.040000000000001</v>
+        <v>5</v>
       </c>
       <c r="X13" s="19">
         <f>V13-Y12</f>
-        <v>7.5000000000002842E-4</v>
+        <v>0</v>
       </c>
       <c r="Y13" s="23">
         <f t="shared" si="1"/>
-        <v>10.039999999999999</v>
+        <v>5</v>
       </c>
       <c r="Z13" s="27"/>
       <c r="AA13" s="24"/>
@@ -2469,7 +2466,7 @@
       <c r="AP13" s="24"/>
       <c r="AQ13" s="24"/>
     </row>
-    <row r="14" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
@@ -2493,15 +2490,15 @@
       </c>
       <c r="S14" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[ga_id],MATCH(U14,TableDay1[es_id],0)),"")</f>
-        <v>800</v>
+        <v/>
       </c>
       <c r="T14" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[brp_id],MATCH(U14,TableDay1[es_id],0)),"")</f>
-        <v>4400000000000</v>
+        <v/>
       </c>
       <c r="U14" s="26" t="str">
         <f>IF(AE$3=0,"",AE$3)</f>
-        <v>4000000000000</v>
+        <v/>
       </c>
       <c r="V14" s="20">
         <f>SUMIFS(TableDay1[TotalHour],TableDay1[es_id],U14,IF(B$2="production",TableDay1[type],TableDay1[settlement_method]),AG$2,TableDay1[resolution],"PT1H")/4</f>
@@ -2588,7 +2585,7 @@
       <c r="CM14" s="2"/>
       <c r="CN14" s="2"/>
     </row>
-    <row r="15" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C15" s="13"/>
       <c r="D15" s="10"/>
       <c r="E15" s="11"/>
@@ -2612,15 +2609,15 @@
       </c>
       <c r="S15" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[ga_id],MATCH(U15,TableDay1[es_id],0)),"")</f>
-        <v>800</v>
+        <v/>
       </c>
       <c r="T15" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[brp_id],MATCH(U15,TableDay1[es_id],0)),"")</f>
-        <v>4400000000000</v>
+        <v/>
       </c>
       <c r="U15" s="26" t="str">
         <f t="shared" ref="U15:V17" si="3">U$14</f>
-        <v>4000000000000</v>
+        <v/>
       </c>
       <c r="V15" s="19">
         <f t="shared" si="3"/>
@@ -2710,7 +2707,7 @@
       <c r="CM15" s="2"/>
       <c r="CN15" s="2"/>
     </row>
-    <row r="16" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C16" s="13"/>
       <c r="D16" s="10"/>
       <c r="E16" s="11"/>
@@ -2734,15 +2731,15 @@
       </c>
       <c r="S16" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[ga_id],MATCH(U16,TableDay1[es_id],0)),"")</f>
-        <v>800</v>
+        <v/>
       </c>
       <c r="T16" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[brp_id],MATCH(U16,TableDay1[es_id],0)),"")</f>
-        <v>4400000000000</v>
+        <v/>
       </c>
       <c r="U16" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>4000000000000</v>
+        <v/>
       </c>
       <c r="V16" s="19">
         <f t="shared" si="3"/>
@@ -2832,7 +2829,7 @@
       <c r="CM16" s="2"/>
       <c r="CN16" s="2"/>
     </row>
-    <row r="17" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="11"/>
@@ -2856,15 +2853,15 @@
       </c>
       <c r="S17" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[ga_id],MATCH(U17,TableDay1[es_id],0)),"")</f>
-        <v>800</v>
+        <v/>
       </c>
       <c r="T17" s="26" t="str">
         <f>_xlfn.IFNA(INDEX(TableDay1[brp_id],MATCH(U17,TableDay1[es_id],0)),"")</f>
-        <v>4400000000000</v>
+        <v/>
       </c>
       <c r="U17" s="26" t="str">
         <f t="shared" si="3"/>
-        <v>4000000000000</v>
+        <v/>
       </c>
       <c r="V17" s="19">
         <f t="shared" si="3"/>
@@ -2950,7 +2947,7 @@
       <c r="CM17" s="2"/>
       <c r="CN17" s="2"/>
     </row>
-    <row r="18" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="11"/>
@@ -3065,7 +3062,7 @@
       <c r="CM18" s="2"/>
       <c r="CN18" s="2"/>
     </row>
-    <row r="19" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="11"/>
@@ -3183,10 +3180,10 @@
       <c r="CM19" s="2"/>
       <c r="CN19" s="2"/>
     </row>
-    <row r="20" spans="1:92" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="E20" s="48" t="str">
         <f>CONCATENATE(B2,"_per_",B1)</f>
-        <v>production_per_ga_brp_es</v>
+        <v>nonprofiled_consumption_per_ga_brp_es</v>
       </c>
       <c r="F20" s="48"/>
       <c r="G20" s="48"/>
@@ -3295,7 +3292,7 @@
       <c r="CM20" s="2"/>
       <c r="CN20" s="2"/>
     </row>
-    <row r="21" spans="1:92" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:92" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B21" s="3" t="s">
         <v>24</v>
       </c>
@@ -3431,7 +3428,7 @@
       <c r="CM21" s="2"/>
       <c r="CN21" s="2"/>
     </row>
-    <row r="22" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:92" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="16" t="str">
         <f>IF(AND(F22&lt;&gt;"null",F22&lt;&gt;""),IF(F22=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G22&lt;&gt;"null",G22&lt;&gt;""),IF(G22=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E22=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
@@ -3439,7 +3436,7 @@
       </c>
       <c r="C22" s="16" t="str">
         <f>IF(AND(F22&lt;&gt;"null",F22&lt;&gt;""),IF(F22=INDEX(TableDay1[es_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(AND(G22&lt;&gt;"null",G22&lt;&gt;""),IF(G22=INDEX(TableDay1[brp_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(E22=INDEX(TableDay1[ga_id],MATCH("SKMP",TableDay1[note],0),1),"skmp","")))</f>
-        <v>skmp</v>
+        <v/>
       </c>
       <c r="D22" s="15" t="s">
         <v>72</v>
@@ -3450,26 +3447,26 @@
       </c>
       <c r="F22" s="31" t="str">
         <f>IF(B$1="ga",IF(E22="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$2=0,"",AE$2),IF(B$1="ga_brp",IF(G22="","","null"))))</f>
-        <v>2000000000000</v>
+        <v>3000000000000</v>
       </c>
       <c r="G22" s="31" t="str">
         <f>IF(B$1="ga",IF(E22="","","null"),IF(B$1="ga_es",IF(F22="","","null"),IF(B$1="ga_brp",IF(AF$2=0,"",AF$2),IF(F22="","",INDEX(TableDay1[brp_id],MATCH(F22,TableDay1[es_id],0),1)))))</f>
-        <v>2200000000000</v>
+        <v>3300000000000</v>
       </c>
       <c r="H22" s="33" t="str">
         <f ca="1">IF(E22="","",SUBSTITUTE(ROUND(I22+J22+K22,3),",","."))</f>
-        <v>10.04</v>
+        <v>7.5</v>
       </c>
       <c r="I22" s="9">
         <f>SUMIFS(Y$10:Y$33,IF(OR(B$1="ga_es",B$1="ga_brp_es"),U$10:U$33,IF(B$1="ga_brp",T$10:T$33,S$10:S$33)),IF(OR(B$1="ga_es",B$1="ga_brp_es"),F22,IF(B$1="ga_brp",G22,E22)),R$10:R$33,D22)</f>
-        <v>10.039999999999999</v>
+        <v>5</v>
       </c>
       <c r="J22" s="9">
         <f ca="1">SUMIFS(INDIRECT(ADDRESS(2,MATCH(D22,$1:$1,0),4,1)&amp;":"&amp;ADDRESS(19,MATCH(D22,$1:$1,0),4,1)),IF(OR(B$1="ga_es",B$1="ga_brp_es"),TableDay1[es_id],IF(B$1="ga_brp",TableDay1[brp_id],TableDay1[ga_id])),IF(OR(B$1="ga_es",B$1="ga_brp_es"),F22,IF(B$1="ga_brp",G22,E22)),IF(B$2="production",TableDay1[type],TableDay1[settlement_method]),AG$2,TableDay1[resolution],"PT15M")</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="K22" s="9">
-        <f t="shared" ref="K22:K45" ca="1" si="5">IF(AND(C22="skmp",B$2="production"),VLOOKUP(D22,D$78:H$81,5,FALSE),IF(AND(B22="glmp",B$2="flex_consumption"),VLOOKUP(D22,D$72:H$75,5,FALSE),0))</f>
+        <f t="shared" ref="K22:K45" si="5">IF(AND(C22="skmp",B$2="production"),VLOOKUP(D22,D$78:H$81,5,FALSE),IF(AND(B22="glmp",B$2="flex_consumption"),VLOOKUP(D22,D$72:H$75,5,FALSE),0))</f>
         <v>0</v>
       </c>
       <c r="L22" s="2"/>
@@ -3574,14 +3571,14 @@
       <c r="CM22" s="2"/>
       <c r="CN22" s="2"/>
     </row>
-    <row r="23" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B23" s="16" t="str">
         <f>IF(AND(F23&lt;&gt;"null",F23&lt;&gt;""),IF(F23=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G23&lt;&gt;"null",G23&lt;&gt;""),IF(G23=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E23=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
       </c>
       <c r="C23" s="16" t="str">
         <f>IF(AND(F23&lt;&gt;"null",F23&lt;&gt;""),IF(F23=INDEX(TableDay1[es_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(AND(G23&lt;&gt;"null",G23&lt;&gt;""),IF(G23=INDEX(TableDay1[brp_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(E23=INDEX(TableDay1[ga_id],MATCH("SKMP",TableDay1[note],0),1),"skmp","")))</f>
-        <v>skmp</v>
+        <v/>
       </c>
       <c r="D23" s="15" t="s">
         <v>73</v>
@@ -3592,26 +3589,26 @@
       </c>
       <c r="F23" s="31" t="str">
         <f>IF(B$1="ga",IF(E23="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$2=0,"",AE$2),IF(B$1="ga_brp",IF(G23="","","null"))))</f>
-        <v>2000000000000</v>
+        <v>3000000000000</v>
       </c>
       <c r="G23" s="31" t="str">
         <f>IF(B$1="ga",IF(E23="","","null"),IF(B$1="ga_es",IF(F23="","","null"),IF(B$1="ga_brp",IF(AF$2=0,"",AF$2),IF(F23="","",INDEX(TableDay1[brp_id],MATCH(F23,TableDay1[es_id],0),1)))))</f>
-        <v>2200000000000</v>
+        <v>3300000000000</v>
       </c>
       <c r="H23" s="33" t="str">
         <f t="shared" ref="H23:H45" ca="1" si="7">IF(E23="","",SUBSTITUTE(ROUND(I23+J23+K23,3),",","."))</f>
-        <v>10.04</v>
+        <v>7.5</v>
       </c>
       <c r="I23" s="9">
         <f t="shared" ref="I23:I45" si="8">SUMIFS(Y$10:Y$33,IF(OR(B$1="ga_es",B$1="ga_brp_es"),U$10:U$33,IF(B$1="ga_brp",T$10:T$33,S$10:S$33)),IF(OR(B$1="ga_es",B$1="ga_brp_es"),F23,IF(B$1="ga_brp",G23,E23)),R$10:R$33,D23)</f>
-        <v>10.039999999999999</v>
+        <v>5</v>
       </c>
       <c r="J23" s="9">
         <f ca="1">SUMIFS(INDIRECT(ADDRESS(2,MATCH(D23,$1:$1,0),4,1)&amp;":"&amp;ADDRESS(19,MATCH(D23,$1:$1,0),4,1)),IF(OR(B$1="ga_es",B$1="ga_brp_es"),TableDay1[es_id],IF(B$1="ga_brp",TableDay1[brp_id],TableDay1[ga_id])),IF(OR(B$1="ga_es",B$1="ga_brp_es"),F23,IF(B$1="ga_brp",G23,E23)),IF(B$2="production",TableDay1[type],TableDay1[settlement_method]),AG$2,TableDay1[resolution],"PT15M")</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="K23" s="9">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L23" s="2"/>
@@ -3719,14 +3716,14 @@
       <c r="CM23" s="2"/>
       <c r="CN23" s="2"/>
     </row>
-    <row r="24" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B24" s="16" t="str">
         <f>IF(AND(F24&lt;&gt;"null",F24&lt;&gt;""),IF(F24=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G24&lt;&gt;"null",G24&lt;&gt;""),IF(G24=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E24=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
       </c>
       <c r="C24" s="16" t="str">
         <f>IF(AND(F24&lt;&gt;"null",F24&lt;&gt;""),IF(F24=INDEX(TableDay1[es_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(AND(G24&lt;&gt;"null",G24&lt;&gt;""),IF(G24=INDEX(TableDay1[brp_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(E24=INDEX(TableDay1[ga_id],MATCH("SKMP",TableDay1[note],0),1),"skmp","")))</f>
-        <v>skmp</v>
+        <v/>
       </c>
       <c r="D24" s="15" t="s">
         <v>74</v>
@@ -3737,26 +3734,26 @@
       </c>
       <c r="F24" s="31" t="str">
         <f>IF(B$1="ga",IF(E24="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$2=0,"",AE$2),IF(B$1="ga_brp",IF(G24="","","null"))))</f>
-        <v>2000000000000</v>
+        <v>3000000000000</v>
       </c>
       <c r="G24" s="31" t="str">
         <f>IF(B$1="ga",IF(E24="","","null"),IF(B$1="ga_es",IF(F24="","","null"),IF(B$1="ga_brp",IF(AF$2=0,"",AF$2),IF(F24="","",INDEX(TableDay1[brp_id],MATCH(F24,TableDay1[es_id],0),1)))))</f>
-        <v>2200000000000</v>
+        <v>3300000000000</v>
       </c>
       <c r="H24" s="33" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>10.039</v>
+        <v>7.5</v>
       </c>
       <c r="I24" s="9">
         <f t="shared" si="8"/>
-        <v>10.039</v>
+        <v>5</v>
       </c>
       <c r="J24" s="9">
         <f ca="1">SUMIFS(INDIRECT(ADDRESS(2,MATCH(D24,$1:$1,0),4,1)&amp;":"&amp;ADDRESS(19,MATCH(D24,$1:$1,0),4,1)),IF(OR(B$1="ga_es",B$1="ga_brp_es"),TableDay1[es_id],IF(B$1="ga_brp",TableDay1[brp_id],TableDay1[ga_id])),IF(OR(B$1="ga_es",B$1="ga_brp_es"),F24,IF(B$1="ga_brp",G24,E24)),IF(B$2="production",TableDay1[type],TableDay1[settlement_method]),AG$2,TableDay1[resolution],"PT15M")</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="K24" s="9">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L24" s="2"/>
@@ -3867,14 +3864,14 @@
       <c r="CM24" s="2"/>
       <c r="CN24" s="2"/>
     </row>
-    <row r="25" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B25" s="16" t="str">
         <f>IF(AND(F25&lt;&gt;"null",F25&lt;&gt;""),IF(F25=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G25&lt;&gt;"null",G25&lt;&gt;""),IF(G25=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E25=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
       </c>
       <c r="C25" s="16" t="str">
         <f>IF(AND(F25&lt;&gt;"null",F25&lt;&gt;""),IF(F25=INDEX(TableDay1[es_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(AND(G25&lt;&gt;"null",G25&lt;&gt;""),IF(G25=INDEX(TableDay1[brp_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(E25=INDEX(TableDay1[ga_id],MATCH("SKMP",TableDay1[note],0),1),"skmp","")))</f>
-        <v>skmp</v>
+        <v/>
       </c>
       <c r="D25" s="15" t="s">
         <v>75</v>
@@ -3885,27 +3882,27 @@
       </c>
       <c r="F25" s="31" t="str">
         <f>IF(B$1="ga",IF(E25="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$2=0,"",AE$2),IF(B$1="ga_brp",IF(G25="","","null"))))</f>
-        <v>2000000000000</v>
+        <v>3000000000000</v>
       </c>
       <c r="G25" s="31" t="str">
         <f>IF(B$1="ga",IF(E25="","","null"),IF(B$1="ga_es",IF(F25="","","null"),IF(B$1="ga_brp",IF(AF$2=0,"",AF$2),IF(F25="","",INDEX(TableDay1[brp_id],MATCH(F25,TableDay1[es_id],0),1)))))</f>
-        <v>2200000000000</v>
+        <v>3300000000000</v>
       </c>
       <c r="H25" s="33" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>14.161</v>
+        <v>15</v>
       </c>
       <c r="I25" s="9">
         <f t="shared" si="8"/>
-        <v>10.039999999999999</v>
+        <v>5</v>
       </c>
       <c r="J25" s="9">
         <f ca="1">SUMIFS(INDIRECT(ADDRESS(2,MATCH(D25,$1:$1,0),4,1)&amp;":"&amp;ADDRESS(19,MATCH(D25,$1:$1,0),4,1)),IF(OR(B$1="ga_es",B$1="ga_brp_es"),TableDay1[es_id],IF(B$1="ga_brp",TableDay1[brp_id],TableDay1[ga_id])),IF(OR(B$1="ga_es",B$1="ga_brp_es"),F25,IF(B$1="ga_brp",G25,E25)),IF(B$2="production",TableDay1[type],TableDay1[settlement_method]),AG$2,TableDay1[resolution],"PT15M")</f>
+        <v>10</v>
+      </c>
+      <c r="K25" s="9">
+        <f t="shared" si="5"/>
         <v>0</v>
-      </c>
-      <c r="K25" s="9">
-        <f t="shared" ca="1" si="5"/>
-        <v>4.1210000000000004</v>
       </c>
       <c r="L25" s="37"/>
       <c r="M25" s="2"/>
@@ -4015,7 +4012,7 @@
       <c r="CM25" s="2"/>
       <c r="CN25" s="2"/>
     </row>
-    <row r="26" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B26" s="16" t="str">
         <f>IF(AND(F26&lt;&gt;"null",F26&lt;&gt;""),IF(F26=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G26&lt;&gt;"null",G26&lt;&gt;""),IF(G26=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E26=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -4029,19 +4026,19 @@
       </c>
       <c r="E26" s="31" t="str">
         <f t="shared" si="6"/>
-        <v>800</v>
+        <v/>
       </c>
       <c r="F26" s="31" t="str">
         <f>IF(B$1="ga",IF(E26="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$3=0,"",AE$3),IF(B$1="ga_brp",IF(G26="","","null"))))</f>
-        <v>4000000000000</v>
+        <v/>
       </c>
       <c r="G26" s="31" t="str">
         <f>IF(B$1="ga",IF(E26="","","null"),IF(B$1="ga_es",IF(F26="","","null"),IF(B$1="ga_brp",IF(AF$3=0,"",AF$3),IF(F26="","",INDEX(TableDay1[brp_id],MATCH(F26,TableDay1[es_id],0),1)))))</f>
-        <v>4400000000000</v>
+        <v/>
       </c>
       <c r="H26" s="33" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v/>
       </c>
       <c r="I26" s="9">
         <f t="shared" si="8"/>
@@ -4157,7 +4154,7 @@
       <c r="CM26" s="2"/>
       <c r="CN26" s="2"/>
     </row>
-    <row r="27" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B27" s="16" t="str">
         <f>IF(AND(F27&lt;&gt;"null",F27&lt;&gt;""),IF(F27=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G27&lt;&gt;"null",G27&lt;&gt;""),IF(G27=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E27=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -4171,19 +4168,19 @@
       </c>
       <c r="E27" s="31" t="str">
         <f t="shared" si="6"/>
-        <v>800</v>
+        <v/>
       </c>
       <c r="F27" s="31" t="str">
         <f>IF(B$1="ga",IF(E27="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$3=0,"",AE$3),IF(B$1="ga_brp",IF(G27="","","null"))))</f>
-        <v>4000000000000</v>
+        <v/>
       </c>
       <c r="G27" s="31" t="str">
         <f>IF(B$1="ga",IF(E27="","","null"),IF(B$1="ga_es",IF(F27="","","null"),IF(B$1="ga_brp",IF(AF$3=0,"",AF$3),IF(F27="","",INDEX(TableDay1[brp_id],MATCH(F27,TableDay1[es_id],0),1)))))</f>
-        <v>4400000000000</v>
+        <v/>
       </c>
       <c r="H27" s="33" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v/>
       </c>
       <c r="I27" s="9">
         <f t="shared" si="8"/>
@@ -4241,11 +4238,11 @@
       <c r="AD27" s="36"/>
       <c r="AE27" s="36" t="str">
         <f>_xlfn.CONCAT("Energy suppliers for "&amp;B2)</f>
-        <v>Energy suppliers for production</v>
+        <v>Energy suppliers for nonprofiled_consumption</v>
       </c>
       <c r="AF27" s="36" t="str">
         <f>_xlfn.CONCAT("Balance responsibles for "&amp;B2)</f>
-        <v>Balance responsibles for production</v>
+        <v>Balance responsibles for nonprofiled_consumption</v>
       </c>
       <c r="AG27" s="36"/>
       <c r="AH27" s="36"/>
@@ -4308,7 +4305,7 @@
       <c r="CM27" s="2"/>
       <c r="CN27" s="2"/>
     </row>
-    <row r="28" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B28" s="16" t="str">
         <f>IF(AND(F28&lt;&gt;"null",F28&lt;&gt;""),IF(F28=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G28&lt;&gt;"null",G28&lt;&gt;""),IF(G28=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E28=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -4322,19 +4319,19 @@
       </c>
       <c r="E28" s="31" t="str">
         <f t="shared" si="6"/>
-        <v>800</v>
+        <v/>
       </c>
       <c r="F28" s="31" t="str">
         <f>IF(B$1="ga",IF(E28="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$3=0,"",AE$3),IF(B$1="ga_brp",IF(G28="","","null"))))</f>
-        <v>4000000000000</v>
+        <v/>
       </c>
       <c r="G28" s="31" t="str">
         <f>IF(B$1="ga",IF(E28="","","null"),IF(B$1="ga_es",IF(F28="","","null"),IF(B$1="ga_brp",IF(AF$3=0,"",AF$3),IF(F28="","",INDEX(TableDay1[brp_id],MATCH(F28,TableDay1[es_id],0),1)))))</f>
-        <v>4400000000000</v>
+        <v/>
       </c>
       <c r="H28" s="33" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v/>
       </c>
       <c r="I28" s="9">
         <f t="shared" si="8"/>
@@ -4459,7 +4456,7 @@
       <c r="CM28" s="2"/>
       <c r="CN28" s="2"/>
     </row>
-    <row r="29" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B29" s="16" t="str">
         <f>IF(AND(F29&lt;&gt;"null",F29&lt;&gt;""),IF(F29=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G29&lt;&gt;"null",G29&lt;&gt;""),IF(G29=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E29=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -4473,19 +4470,19 @@
       </c>
       <c r="E29" s="31" t="str">
         <f t="shared" si="6"/>
-        <v>800</v>
+        <v/>
       </c>
       <c r="F29" s="31" t="str">
         <f>IF(B$1="ga",IF(E29="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$3=0,"",AE$3),IF(B$1="ga_brp",IF(G29="","","null"))))</f>
-        <v>4000000000000</v>
+        <v/>
       </c>
       <c r="G29" s="31" t="str">
         <f>IF(B$1="ga",IF(E29="","","null"),IF(B$1="ga_es",IF(F29="","","null"),IF(B$1="ga_brp",IF(AF$3=0,"",AF$3),IF(F29="","",INDEX(TableDay1[brp_id],MATCH(F29,TableDay1[es_id],0),1)))))</f>
-        <v>4400000000000</v>
+        <v/>
       </c>
       <c r="H29" s="33" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v/>
       </c>
       <c r="I29" s="9">
         <f t="shared" si="8"/>
@@ -4538,11 +4535,11 @@
       <c r="AD29" s="36"/>
       <c r="AE29" s="36" t="str" cm="1">
         <f t="array" ref="AE29">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE14)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE14)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
-        <v>2000000000000</v>
+        <v/>
       </c>
       <c r="AF29" s="36" t="str" cm="1">
         <f t="array" ref="AF29">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[brp_id]=AF14)*(TableDay1[type]=$AG$2),""),,10)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[brp_id]=AF14)*(TableDay1[settlement_method]=AG$2),""),,10))),"")</f>
-        <v>2200000000000</v>
+        <v/>
       </c>
       <c r="AG29" s="36"/>
       <c r="AH29" s="36"/>
@@ -4605,7 +4602,7 @@
       <c r="CM29" s="2"/>
       <c r="CN29" s="2"/>
     </row>
-    <row r="30" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B30" s="16" t="str">
         <f>IF(AND(F30&lt;&gt;"null",F30&lt;&gt;""),IF(F30=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G30&lt;&gt;"null",G30&lt;&gt;""),IF(G30=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E30=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -4681,11 +4678,11 @@
       <c r="AD30" s="36"/>
       <c r="AE30" s="36" t="str" cm="1">
         <f t="array" ref="AE30">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE15)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE15)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
-        <v/>
+        <v>3000000000000</v>
       </c>
       <c r="AF30" s="36" t="str" cm="1">
         <f t="array" ref="AF30">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[brp_id]=AF15)*(TableDay1[type]=$AG$2),""),,10)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[brp_id]=AF15)*(TableDay1[settlement_method]=AG$2),""),,10))),"")</f>
-        <v/>
+        <v>3300000000000</v>
       </c>
       <c r="AG30" s="36"/>
       <c r="AH30" s="36"/>
@@ -4748,7 +4745,7 @@
       <c r="CM30" s="2"/>
       <c r="CN30" s="2"/>
     </row>
-    <row r="31" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B31" s="16" t="str">
         <f>IF(AND(F31&lt;&gt;"null",F31&lt;&gt;""),IF(F31=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G31&lt;&gt;"null",G31&lt;&gt;""),IF(G31=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E31=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -4827,11 +4824,11 @@
       <c r="AD31" s="36"/>
       <c r="AE31" s="36" t="str" cm="1">
         <f t="array" ref="AE31">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE16)*(TableDay1[type]="E18"),""),,9)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[es_id]=AE16)*(TableDay1[settlement_method]=AG$2),""),,9))),"")</f>
-        <v>4000000000000</v>
+        <v/>
       </c>
       <c r="AF31" s="36" t="str" cm="1">
         <f t="array" ref="AF31">IFERROR(IF($B$2="production",_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[brp_id]=AF16)*(TableDay1[type]=$AG$2),""),,10)),_xlfn.UNIQUE(INDEX(_xlfn._xlws.FILTER(TableDay1[[type]:[brp_id]],(TableDay1[brp_id]=AF16)*(TableDay1[settlement_method]=AG$2),""),,10))),"")</f>
-        <v>4400000000000</v>
+        <v/>
       </c>
       <c r="AG31" s="36"/>
       <c r="AH31" s="36"/>
@@ -4894,7 +4891,7 @@
       <c r="CM31" s="2"/>
       <c r="CN31" s="2"/>
     </row>
-    <row r="32" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B32" s="16" t="str">
         <f>IF(AND(F32&lt;&gt;"null",F32&lt;&gt;""),IF(F32=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G32&lt;&gt;"null",G32&lt;&gt;""),IF(G32=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E32=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -5040,7 +5037,7 @@
       <c r="CM32" s="2"/>
       <c r="CN32" s="2"/>
     </row>
-    <row r="33" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B33" s="16" t="str">
         <f>IF(AND(F33&lt;&gt;"null",F33&lt;&gt;""),IF(F33=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G33&lt;&gt;"null",G33&lt;&gt;""),IF(G33=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E33=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -5180,7 +5177,7 @@
       <c r="CM33" s="2"/>
       <c r="CN33" s="2"/>
     </row>
-    <row r="34" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B34" s="16" t="str">
         <f>IF(AND(F34&lt;&gt;"null",F34&lt;&gt;""),IF(F34=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G34&lt;&gt;"null",G34&lt;&gt;""),IF(G34=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E34=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -5297,7 +5294,7 @@
       <c r="CM34" s="2"/>
       <c r="CN34" s="2"/>
     </row>
-    <row r="35" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B35" s="16" t="str">
         <f>IF(AND(F35&lt;&gt;"null",F35&lt;&gt;""),IF(F35=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G35&lt;&gt;"null",G35&lt;&gt;""),IF(G35=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E35=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -5425,7 +5422,7 @@
       <c r="CM35" s="2"/>
       <c r="CN35" s="2"/>
     </row>
-    <row r="36" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B36" s="16" t="str">
         <f>IF(AND(F36&lt;&gt;"null",F36&lt;&gt;""),IF(F36=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G36&lt;&gt;"null",G36&lt;&gt;""),IF(G36=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E36=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -5555,7 +5552,7 @@
       <c r="CM36" s="2"/>
       <c r="CN36" s="2"/>
     </row>
-    <row r="37" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B37" s="16" t="str">
         <f>IF(AND(F37&lt;&gt;"null",F37&lt;&gt;""),IF(F37=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G37&lt;&gt;"null",G37&lt;&gt;""),IF(G37=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E37=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -5686,7 +5683,7 @@
       <c r="CM37" s="2"/>
       <c r="CN37" s="2"/>
     </row>
-    <row r="38" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B38" s="16" t="str">
         <f>IF(AND(F38&lt;&gt;"null",F38&lt;&gt;""),IF(F38=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G38&lt;&gt;"null",G38&lt;&gt;""),IF(G38=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E38=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -5820,7 +5817,7 @@
       <c r="CM38" s="2"/>
       <c r="CN38" s="2"/>
     </row>
-    <row r="39" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B39" s="16" t="str">
         <f>IF(AND(F39&lt;&gt;"null",F39&lt;&gt;""),IF(F39=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G39&lt;&gt;"null",G39&lt;&gt;""),IF(G39=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E39=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -5954,7 +5951,7 @@
       <c r="CM39" s="2"/>
       <c r="CN39" s="2"/>
     </row>
-    <row r="40" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B40" s="16" t="str">
         <f>IF(AND(F40&lt;&gt;"null",F40&lt;&gt;""),IF(F40=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G40&lt;&gt;"null",G40&lt;&gt;""),IF(G40=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E40=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -6088,7 +6085,7 @@
       <c r="CM40" s="2"/>
       <c r="CN40" s="2"/>
     </row>
-    <row r="41" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B41" s="16" t="str">
         <f>IF(AND(F41&lt;&gt;"null",F41&lt;&gt;""),IF(F41=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G41&lt;&gt;"null",G41&lt;&gt;""),IF(G41=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E41=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -6216,7 +6213,7 @@
       <c r="CM41" s="2"/>
       <c r="CN41" s="2"/>
     </row>
-    <row r="42" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B42" s="16" t="str">
         <f>IF(AND(F42&lt;&gt;"null",F42&lt;&gt;""),IF(F42=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G42&lt;&gt;"null",G42&lt;&gt;""),IF(G42=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E42=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -6346,7 +6343,7 @@
       <c r="CM42" s="2"/>
       <c r="CN42" s="2"/>
     </row>
-    <row r="43" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B43" s="16" t="str">
         <f>IF(AND(F43&lt;&gt;"null",F43&lt;&gt;""),IF(F43=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G43&lt;&gt;"null",G43&lt;&gt;""),IF(G43=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E43=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -6477,7 +6474,7 @@
       <c r="CM43" s="2"/>
       <c r="CN43" s="2"/>
     </row>
-    <row r="44" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B44" s="16" t="str">
         <f>IF(AND(F44&lt;&gt;"null",F44&lt;&gt;""),IF(F44=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G44&lt;&gt;"null",G44&lt;&gt;""),IF(G44=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E44=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -6611,7 +6608,7 @@
       <c r="CM44" s="2"/>
       <c r="CN44" s="2"/>
     </row>
-    <row r="45" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B45" s="16" t="str">
         <f>IF(AND(F45&lt;&gt;"null",F45&lt;&gt;""),IF(F45=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G45&lt;&gt;"null",G45&lt;&gt;""),IF(G45=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E45=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
         <v/>
@@ -6745,7 +6742,7 @@
       <c r="CM45" s="2"/>
       <c r="CN45" s="2"/>
     </row>
-    <row r="46" spans="1:92" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C46" s="2"/>
       <c r="E46" s="48" t="s">
         <v>33</v>
@@ -6846,7 +6843,7 @@
       <c r="CM46" s="2"/>
       <c r="CN46" s="2"/>
     </row>
-    <row r="47" spans="1:92" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:92" ht="18.5" x14ac:dyDescent="0.45">
       <c r="C47" s="2"/>
       <c r="D47" s="4" t="s">
         <v>20</v>
@@ -6950,7 +6947,7 @@
       <c r="CM47" s="2"/>
       <c r="CN47" s="2"/>
     </row>
-    <row r="48" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:92" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -7065,7 +7062,7 @@
       <c r="CM48" s="2"/>
       <c r="CN48" s="2"/>
     </row>
-    <row r="49" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:92" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -7181,7 +7178,7 @@
       <c r="CM49" s="2"/>
       <c r="CN49" s="2"/>
     </row>
-    <row r="50" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:92" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -7300,7 +7297,7 @@
       <c r="CM50" s="2"/>
       <c r="CN50" s="2"/>
     </row>
-    <row r="51" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:92" x14ac:dyDescent="0.35">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -7419,7 +7416,7 @@
       <c r="CM51" s="2"/>
       <c r="CN51" s="2"/>
     </row>
-    <row r="52" spans="1:92" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -7522,7 +7519,7 @@
       <c r="CM52" s="2"/>
       <c r="CN52" s="2"/>
     </row>
-    <row r="53" spans="1:92" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:92" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -7628,7 +7625,7 @@
       <c r="CM53" s="2"/>
       <c r="CN53" s="2"/>
     </row>
-    <row r="54" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:92" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -7743,7 +7740,7 @@
       <c r="CM54" s="2"/>
       <c r="CN54" s="2"/>
     </row>
-    <row r="55" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:92" x14ac:dyDescent="0.35">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -7858,7 +7855,7 @@
       <c r="CM55" s="2"/>
       <c r="CN55" s="2"/>
     </row>
-    <row r="56" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:92" x14ac:dyDescent="0.35">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -7976,7 +7973,7 @@
       <c r="CM56" s="2"/>
       <c r="CN56" s="2"/>
     </row>
-    <row r="57" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:92" x14ac:dyDescent="0.35">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -8094,7 +8091,7 @@
       <c r="CM57" s="2"/>
       <c r="CN57" s="2"/>
     </row>
-    <row r="58" spans="1:92" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -8197,7 +8194,7 @@
       <c r="CM58" s="2"/>
       <c r="CN58" s="2"/>
     </row>
-    <row r="59" spans="1:92" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:92" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -8303,7 +8300,7 @@
       <c r="CM59" s="2"/>
       <c r="CN59" s="2"/>
     </row>
-    <row r="60" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C60" s="2"/>
       <c r="D60" s="8" t="s">
         <v>3</v>
@@ -8415,7 +8412,7 @@
       <c r="CM60" s="2"/>
       <c r="CN60" s="2"/>
     </row>
-    <row r="61" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C61" s="2"/>
       <c r="D61" s="8" t="s">
         <v>4</v>
@@ -8528,7 +8525,7 @@
       <c r="CM61" s="2"/>
       <c r="CN61" s="2"/>
     </row>
-    <row r="62" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C62" s="2"/>
       <c r="D62" s="8" t="s">
         <v>5</v>
@@ -8644,7 +8641,7 @@
       <c r="CM62" s="2"/>
       <c r="CN62" s="2"/>
     </row>
-    <row r="63" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C63" s="2"/>
       <c r="D63" s="8" t="s">
         <v>6</v>
@@ -8760,7 +8757,7 @@
       <c r="CM63" s="2"/>
       <c r="CN63" s="2"/>
     </row>
-    <row r="64" spans="1:92" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C64" s="2"/>
       <c r="E64" s="52" t="s">
         <v>37</v>
@@ -8861,7 +8858,7 @@
       <c r="CM64" s="2"/>
       <c r="CN64" s="2"/>
     </row>
-    <row r="65" spans="3:92" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:92" ht="18.5" x14ac:dyDescent="0.45">
       <c r="C65" s="2"/>
       <c r="D65" s="4" t="s">
         <v>20</v>
@@ -8965,7 +8962,7 @@
       <c r="CM65" s="2"/>
       <c r="CN65" s="2"/>
     </row>
-    <row r="66" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C66" s="2"/>
       <c r="D66" s="8" t="s">
         <v>3</v>
@@ -9077,7 +9074,7 @@
       <c r="CM66" s="2"/>
       <c r="CN66" s="2"/>
     </row>
-    <row r="67" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C67" s="2"/>
       <c r="D67" s="8" t="s">
         <v>4</v>
@@ -9190,7 +9187,7 @@
       <c r="CM67" s="2"/>
       <c r="CN67" s="2"/>
     </row>
-    <row r="68" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C68" s="2"/>
       <c r="D68" s="8" t="s">
         <v>5</v>
@@ -9306,7 +9303,7 @@
       <c r="CM68" s="2"/>
       <c r="CN68" s="2"/>
     </row>
-    <row r="69" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C69" s="2"/>
       <c r="D69" s="8" t="s">
         <v>6</v>
@@ -9423,7 +9420,7 @@
       <c r="CM69" s="2"/>
       <c r="CN69" s="2"/>
     </row>
-    <row r="70" spans="3:92" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C70" s="2"/>
       <c r="E70" s="52" t="s">
         <v>39</v>
@@ -9524,7 +9521,7 @@
       <c r="CM70" s="2"/>
       <c r="CN70" s="2"/>
     </row>
-    <row r="71" spans="3:92" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:92" ht="18.5" x14ac:dyDescent="0.45">
       <c r="C71" s="2"/>
       <c r="D71" s="4" t="s">
         <v>20</v>
@@ -9617,7 +9614,7 @@
       <c r="CM71" s="2"/>
       <c r="CN71" s="2"/>
     </row>
-    <row r="72" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C72" s="2"/>
       <c r="D72" s="15" t="s">
         <v>75</v>
@@ -9716,7 +9713,7 @@
       <c r="CM72" s="2"/>
       <c r="CN72" s="2"/>
     </row>
-    <row r="73" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C73" s="2"/>
       <c r="D73" s="15" t="s">
         <v>74</v>
@@ -9808,7 +9805,7 @@
       <c r="CM73" s="2"/>
       <c r="CN73" s="2"/>
     </row>
-    <row r="74" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C74" s="2"/>
       <c r="D74" s="15" t="s">
         <v>73</v>
@@ -9911,7 +9908,7 @@
       <c r="CM74" s="2"/>
       <c r="CN74" s="2"/>
     </row>
-    <row r="75" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C75" s="2"/>
       <c r="D75" s="15" t="s">
         <v>72</v>
@@ -10012,7 +10009,7 @@
       <c r="CM75" s="2"/>
       <c r="CN75" s="2"/>
     </row>
-    <row r="76" spans="3:92" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C76" s="2"/>
       <c r="E76" s="52" t="s">
         <v>40</v>
@@ -10105,7 +10102,7 @@
       <c r="CM76" s="2"/>
       <c r="CN76" s="2"/>
     </row>
-    <row r="77" spans="3:92" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:92" ht="18.5" x14ac:dyDescent="0.45">
       <c r="C77" s="2"/>
       <c r="D77" s="4" t="s">
         <v>20</v>
@@ -10207,7 +10204,7 @@
       <c r="CM77" s="2"/>
       <c r="CN77" s="2"/>
     </row>
-    <row r="78" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C78" s="2"/>
       <c r="D78" s="15" t="s">
         <v>75</v>
@@ -10314,7 +10311,7 @@
       <c r="CM78" s="2"/>
       <c r="CN78" s="2"/>
     </row>
-    <row r="79" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C79" s="2"/>
       <c r="D79" s="15" t="s">
         <v>74</v>
@@ -10421,7 +10418,7 @@
       <c r="CM79" s="2"/>
       <c r="CN79" s="2"/>
     </row>
-    <row r="80" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C80" s="2"/>
       <c r="D80" s="15" t="s">
         <v>73</v>
@@ -10528,7 +10525,7 @@
       <c r="CM80" s="2"/>
       <c r="CN80" s="2"/>
     </row>
-    <row r="81" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C81" s="2"/>
       <c r="D81" s="15" t="s">
         <v>72</v>
@@ -10635,7 +10632,7 @@
       <c r="CM81" s="2"/>
       <c r="CN81" s="2"/>
     </row>
-    <row r="82" spans="3:92" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C82" s="2"/>
       <c r="E82" s="52" t="s">
         <v>77</v>
@@ -10728,7 +10725,7 @@
       <c r="CM82" s="2"/>
       <c r="CN82" s="2"/>
     </row>
-    <row r="83" spans="3:92" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:92" ht="18.5" x14ac:dyDescent="0.45">
       <c r="C83" s="2"/>
       <c r="D83" s="4" t="s">
         <v>20</v>
@@ -10830,7 +10827,7 @@
       <c r="CM83" s="2"/>
       <c r="CN83" s="2"/>
     </row>
-    <row r="84" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C84" s="2"/>
       <c r="D84" s="15" t="s">
         <v>72</v>
@@ -10929,7 +10926,7 @@
       <c r="CM84" s="2"/>
       <c r="CN84" s="2"/>
     </row>
-    <row r="85" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C85" s="2"/>
       <c r="D85" s="15" t="s">
         <v>73</v>
@@ -11036,7 +11033,7 @@
       <c r="CM85" s="2"/>
       <c r="CN85" s="2"/>
     </row>
-    <row r="86" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C86" s="2"/>
       <c r="D86" s="15" t="s">
         <v>74</v>
@@ -11147,7 +11144,7 @@
       <c r="CM86" s="2"/>
       <c r="CN86" s="2"/>
     </row>
-    <row r="87" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C87" s="2"/>
       <c r="D87" s="15" t="s">
         <v>75</v>
@@ -11263,7 +11260,7 @@
       <c r="CM87" s="2"/>
       <c r="CN87" s="2"/>
     </row>
-    <row r="88" spans="3:92" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C88" s="2"/>
       <c r="E88" s="52" t="s">
         <v>78</v>
@@ -11365,7 +11362,7 @@
       <c r="CM88" s="2"/>
       <c r="CN88" s="2"/>
     </row>
-    <row r="89" spans="3:92" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:92" ht="18.5" x14ac:dyDescent="0.45">
       <c r="C89" s="2"/>
       <c r="D89" s="4" t="s">
         <v>20</v>
@@ -11383,7 +11380,7 @@
         <v>2</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="J89" s="2"/>
       <c r="R89" s="2"/>
@@ -11478,7 +11475,7 @@
       <c r="CM89" s="2"/>
       <c r="CN89" s="2"/>
     </row>
-    <row r="90" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C90" s="2"/>
       <c r="D90" s="15" t="s">
         <v>72</v>
@@ -11596,7 +11593,7 @@
       <c r="CM90" s="2"/>
       <c r="CN90" s="2"/>
     </row>
-    <row r="91" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C91" s="2"/>
       <c r="D91" s="15" t="s">
         <v>73</v>
@@ -11716,7 +11713,7 @@
       <c r="CM91" s="2"/>
       <c r="CN91" s="2"/>
     </row>
-    <row r="92" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C92" s="2"/>
       <c r="D92" s="15" t="s">
         <v>74</v>
@@ -11835,7 +11832,7 @@
       <c r="CM92" s="2"/>
       <c r="CN92" s="2"/>
     </row>
-    <row r="93" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C93" s="2"/>
       <c r="D93" s="15" t="s">
         <v>75</v>
@@ -11954,7 +11951,7 @@
       <c r="CM93" s="2"/>
       <c r="CN93" s="2"/>
     </row>
-    <row r="94" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C94" s="2"/>
       <c r="D94" s="15" t="s">
         <v>72</v>
@@ -12070,7 +12067,7 @@
       <c r="CM94" s="2"/>
       <c r="CN94" s="2"/>
     </row>
-    <row r="95" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C95" s="2"/>
       <c r="D95" s="15" t="s">
         <v>73</v>
@@ -12189,7 +12186,7 @@
       <c r="CM95" s="2"/>
       <c r="CN95" s="2"/>
     </row>
-    <row r="96" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C96" s="2"/>
       <c r="D96" s="15" t="s">
         <v>74</v>
@@ -12308,7 +12305,7 @@
       <c r="CM96" s="2"/>
       <c r="CN96" s="2"/>
     </row>
-    <row r="97" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C97" s="2"/>
       <c r="D97" s="15" t="s">
         <v>75</v>
@@ -12427,7 +12424,7 @@
       <c r="CM97" s="2"/>
       <c r="CN97" s="2"/>
     </row>
-    <row r="98" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C98" s="2"/>
       <c r="D98" s="15" t="s">
         <v>72</v>
@@ -12543,7 +12540,7 @@
       <c r="CM98" s="2"/>
       <c r="CN98" s="2"/>
     </row>
-    <row r="99" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C99" s="2"/>
       <c r="D99" s="15" t="s">
         <v>73</v>
@@ -12662,7 +12659,7 @@
       <c r="CM99" s="2"/>
       <c r="CN99" s="2"/>
     </row>
-    <row r="100" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C100" s="2"/>
       <c r="D100" s="15" t="s">
         <v>74</v>
@@ -12781,7 +12778,7 @@
       <c r="CM100" s="2"/>
       <c r="CN100" s="2"/>
     </row>
-    <row r="101" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C101" s="2"/>
       <c r="D101" s="15" t="s">
         <v>75</v>
@@ -12900,7 +12897,7 @@
       <c r="CM101" s="2"/>
       <c r="CN101" s="2"/>
     </row>
-    <row r="102" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C102" s="2"/>
       <c r="D102" s="15" t="s">
         <v>72</v>
@@ -13016,7 +13013,7 @@
       <c r="CM102" s="2"/>
       <c r="CN102" s="2"/>
     </row>
-    <row r="103" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C103" s="2"/>
       <c r="D103" s="15" t="s">
         <v>73</v>
@@ -13135,7 +13132,7 @@
       <c r="CM103" s="2"/>
       <c r="CN103" s="2"/>
     </row>
-    <row r="104" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C104" s="2"/>
       <c r="D104" s="15" t="s">
         <v>74</v>
@@ -13254,7 +13251,7 @@
       <c r="CM104" s="2"/>
       <c r="CN104" s="2"/>
     </row>
-    <row r="105" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C105" s="2"/>
       <c r="D105" s="15" t="s">
         <v>75</v>
@@ -13373,7 +13370,7 @@
       <c r="CM105" s="2"/>
       <c r="CN105" s="2"/>
     </row>
-    <row r="106" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C106" s="2"/>
       <c r="D106" s="15" t="s">
         <v>72</v>
@@ -13489,7 +13486,7 @@
       <c r="CM106" s="2"/>
       <c r="CN106" s="2"/>
     </row>
-    <row r="107" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C107" s="2"/>
       <c r="D107" s="15" t="s">
         <v>73</v>
@@ -13608,7 +13605,7 @@
       <c r="CM107" s="2"/>
       <c r="CN107" s="2"/>
     </row>
-    <row r="108" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C108" s="2"/>
       <c r="D108" s="15" t="s">
         <v>74</v>
@@ -13727,7 +13724,7 @@
       <c r="CM108" s="2"/>
       <c r="CN108" s="2"/>
     </row>
-    <row r="109" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C109" s="2"/>
       <c r="D109" s="15" t="s">
         <v>75</v>
@@ -13846,7 +13843,7 @@
       <c r="CM109" s="2"/>
       <c r="CN109" s="2"/>
     </row>
-    <row r="110" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C110" s="2"/>
       <c r="D110" s="15" t="s">
         <v>72</v>
@@ -13958,7 +13955,7 @@
       <c r="CM110" s="2"/>
       <c r="CN110" s="2"/>
     </row>
-    <row r="111" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C111" s="2"/>
       <c r="D111" s="15" t="s">
         <v>73</v>
@@ -14070,7 +14067,7 @@
       <c r="CM111" s="2"/>
       <c r="CN111" s="2"/>
     </row>
-    <row r="112" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C112" s="2"/>
       <c r="D112" s="15" t="s">
         <v>74</v>
@@ -14182,7 +14179,7 @@
       <c r="CM112" s="2"/>
       <c r="CN112" s="2"/>
     </row>
-    <row r="113" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C113" s="2"/>
       <c r="D113" s="15" t="s">
         <v>75</v>
@@ -14294,7 +14291,7 @@
       <c r="CM113" s="2"/>
       <c r="CN113" s="2"/>
     </row>
-    <row r="114" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C114" s="2"/>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
@@ -14384,7 +14381,7 @@
       <c r="CM114" s="2"/>
       <c r="CN114" s="2"/>
     </row>
-    <row r="115" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C115" s="2"/>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
@@ -14474,7 +14471,7 @@
       <c r="CM115" s="2"/>
       <c r="CN115" s="2"/>
     </row>
-    <row r="116" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C116" s="2"/>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
@@ -14564,7 +14561,7 @@
       <c r="CM116" s="2"/>
       <c r="CN116" s="2"/>
     </row>
-    <row r="117" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C117" s="2"/>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
@@ -14654,7 +14651,7 @@
       <c r="CM117" s="2"/>
       <c r="CN117" s="2"/>
     </row>
-    <row r="118" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
@@ -14746,7 +14743,7 @@
       <c r="CM118" s="2"/>
       <c r="CN118" s="2"/>
     </row>
-    <row r="119" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
@@ -14838,7 +14835,7 @@
       <c r="CM119" s="2"/>
       <c r="CN119" s="2"/>
     </row>
-    <row r="120" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
@@ -14930,7 +14927,7 @@
       <c r="CM120" s="2"/>
       <c r="CN120" s="2"/>
     </row>
-    <row r="121" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
@@ -15022,7 +15019,7 @@
       <c r="CM121" s="2"/>
       <c r="CN121" s="2"/>
     </row>
-    <row r="122" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
@@ -15114,7 +15111,7 @@
       <c r="CM122" s="2"/>
       <c r="CN122" s="2"/>
     </row>
-    <row r="123" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
@@ -15206,7 +15203,7 @@
       <c r="CM123" s="2"/>
       <c r="CN123" s="2"/>
     </row>
-    <row r="124" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
@@ -15298,7 +15295,7 @@
       <c r="CM124" s="2"/>
       <c r="CN124" s="2"/>
     </row>
-    <row r="125" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
@@ -15390,7 +15387,7 @@
       <c r="CM125" s="2"/>
       <c r="CN125" s="2"/>
     </row>
-    <row r="126" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
@@ -15482,7 +15479,7 @@
       <c r="CM126" s="2"/>
       <c r="CN126" s="2"/>
     </row>
-    <row r="127" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="127" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
@@ -15574,7 +15571,7 @@
       <c r="CM127" s="2"/>
       <c r="CN127" s="2"/>
     </row>
-    <row r="128" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
@@ -15666,7 +15663,7 @@
       <c r="CM128" s="2"/>
       <c r="CN128" s="2"/>
     </row>
-    <row r="129" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
@@ -15758,7 +15755,7 @@
       <c r="CM129" s="2"/>
       <c r="CN129" s="2"/>
     </row>
-    <row r="130" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="130" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
@@ -15850,7 +15847,7 @@
       <c r="CM130" s="2"/>
       <c r="CN130" s="2"/>
     </row>
-    <row r="131" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="131" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
@@ -15942,7 +15939,7 @@
       <c r="CM131" s="2"/>
       <c r="CN131" s="2"/>
     </row>
-    <row r="132" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="132" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
@@ -16034,7 +16031,7 @@
       <c r="CM132" s="2"/>
       <c r="CN132" s="2"/>
     </row>
-    <row r="133" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="133" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
@@ -16126,7 +16123,7 @@
       <c r="CM133" s="2"/>
       <c r="CN133" s="2"/>
     </row>
-    <row r="134" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="134" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
@@ -16218,7 +16215,7 @@
       <c r="CM134" s="2"/>
       <c r="CN134" s="2"/>
     </row>
-    <row r="135" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="135" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
@@ -16310,7 +16307,7 @@
       <c r="CM135" s="2"/>
       <c r="CN135" s="2"/>
     </row>
-    <row r="136" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="136" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
       <c r="E136" s="2"/>
@@ -16402,7 +16399,7 @@
       <c r="CM136" s="2"/>
       <c r="CN136" s="2"/>
     </row>
-    <row r="137" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="137" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
       <c r="E137" s="2"/>
@@ -16494,7 +16491,7 @@
       <c r="CM137" s="2"/>
       <c r="CN137" s="2"/>
     </row>
-    <row r="138" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="138" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
@@ -16586,7 +16583,7 @@
       <c r="CM138" s="2"/>
       <c r="CN138" s="2"/>
     </row>
-    <row r="139" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="139" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
@@ -16678,7 +16675,7 @@
       <c r="CM139" s="2"/>
       <c r="CN139" s="2"/>
     </row>
-    <row r="140" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="140" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
       <c r="E140" s="2"/>
@@ -16770,7 +16767,7 @@
       <c r="CM140" s="2"/>
       <c r="CN140" s="2"/>
     </row>
-    <row r="141" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="141" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
       <c r="E141" s="2"/>
@@ -16862,7 +16859,7 @@
       <c r="CM141" s="2"/>
       <c r="CN141" s="2"/>
     </row>
-    <row r="142" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="142" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
@@ -16954,7 +16951,7 @@
       <c r="CM142" s="2"/>
       <c r="CN142" s="2"/>
     </row>
-    <row r="143" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="143" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
       <c r="E143" s="2"/>
@@ -17046,7 +17043,7 @@
       <c r="CM143" s="2"/>
       <c r="CN143" s="2"/>
     </row>
-    <row r="144" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="144" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
@@ -17138,7 +17135,7 @@
       <c r="CM144" s="2"/>
       <c r="CN144" s="2"/>
     </row>
-    <row r="145" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
@@ -17230,7 +17227,7 @@
       <c r="CM145" s="2"/>
       <c r="CN145" s="2"/>
     </row>
-    <row r="146" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="146" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
@@ -17322,7 +17319,7 @@
       <c r="CM146" s="2"/>
       <c r="CN146" s="2"/>
     </row>
-    <row r="147" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="147" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
@@ -17414,7 +17411,7 @@
       <c r="CM147" s="2"/>
       <c r="CN147" s="2"/>
     </row>
-    <row r="148" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="148" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
@@ -17506,7 +17503,7 @@
       <c r="CM148" s="2"/>
       <c r="CN148" s="2"/>
     </row>
-    <row r="149" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="149" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
@@ -17598,7 +17595,7 @@
       <c r="CM149" s="2"/>
       <c r="CN149" s="2"/>
     </row>
-    <row r="150" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="150" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C150" s="2"/>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
@@ -17690,7 +17687,7 @@
       <c r="CM150" s="2"/>
       <c r="CN150" s="2"/>
     </row>
-    <row r="151" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="151" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C151" s="2"/>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
@@ -17782,7 +17779,7 @@
       <c r="CM151" s="2"/>
       <c r="CN151" s="2"/>
     </row>
-    <row r="152" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="152" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
@@ -17874,7 +17871,7 @@
       <c r="CM152" s="2"/>
       <c r="CN152" s="2"/>
     </row>
-    <row r="153" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="153" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C153" s="2"/>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
@@ -17966,7 +17963,7 @@
       <c r="CM153" s="2"/>
       <c r="CN153" s="2"/>
     </row>
-    <row r="154" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="154" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C154" s="2"/>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
@@ -18058,7 +18055,7 @@
       <c r="CM154" s="2"/>
       <c r="CN154" s="2"/>
     </row>
-    <row r="155" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C155" s="2"/>
       <c r="D155" s="2"/>
       <c r="E155" s="2"/>
@@ -18150,7 +18147,7 @@
       <c r="CM155" s="2"/>
       <c r="CN155" s="2"/>
     </row>
-    <row r="156" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="156" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C156" s="2"/>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
@@ -18242,7 +18239,7 @@
       <c r="CM156" s="2"/>
       <c r="CN156" s="2"/>
     </row>
-    <row r="157" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="157" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C157" s="2"/>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
@@ -18334,7 +18331,7 @@
       <c r="CM157" s="2"/>
       <c r="CN157" s="2"/>
     </row>
-    <row r="158" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="158" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C158" s="2"/>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
@@ -18426,7 +18423,7 @@
       <c r="CM158" s="2"/>
       <c r="CN158" s="2"/>
     </row>
-    <row r="159" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="159" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C159" s="2"/>
       <c r="D159" s="2"/>
       <c r="E159" s="2"/>
@@ -18518,7 +18515,7 @@
       <c r="CM159" s="2"/>
       <c r="CN159" s="2"/>
     </row>
-    <row r="160" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="160" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C160" s="2"/>
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
@@ -18610,7 +18607,7 @@
       <c r="CM160" s="2"/>
       <c r="CN160" s="2"/>
     </row>
-    <row r="161" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C161" s="2"/>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
@@ -18702,7 +18699,7 @@
       <c r="CM161" s="2"/>
       <c r="CN161" s="2"/>
     </row>
-    <row r="162" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C162" s="2"/>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
@@ -18794,7 +18791,7 @@
       <c r="CM162" s="2"/>
       <c r="CN162" s="2"/>
     </row>
-    <row r="163" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
@@ -18886,7 +18883,7 @@
       <c r="CM163" s="2"/>
       <c r="CN163" s="2"/>
     </row>
-    <row r="164" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
@@ -18978,7 +18975,7 @@
       <c r="CM164" s="2"/>
       <c r="CN164" s="2"/>
     </row>
-    <row r="165" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C165" s="2"/>
       <c r="D165" s="2"/>
       <c r="E165" s="2"/>
@@ -19070,7 +19067,7 @@
       <c r="CM165" s="2"/>
       <c r="CN165" s="2"/>
     </row>
-    <row r="166" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C166" s="2"/>
       <c r="D166" s="2"/>
       <c r="E166" s="2"/>
@@ -19162,7 +19159,7 @@
       <c r="CM166" s="2"/>
       <c r="CN166" s="2"/>
     </row>
-    <row r="167" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C167" s="2"/>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
@@ -19254,7 +19251,7 @@
       <c r="CM167" s="2"/>
       <c r="CN167" s="2"/>
     </row>
-    <row r="168" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C168" s="2"/>
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
@@ -19346,7 +19343,7 @@
       <c r="CM168" s="2"/>
       <c r="CN168" s="2"/>
     </row>
-    <row r="169" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
       <c r="E169" s="2"/>
@@ -19438,7 +19435,7 @@
       <c r="CM169" s="2"/>
       <c r="CN169" s="2"/>
     </row>
-    <row r="170" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C170" s="2"/>
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
@@ -19530,7 +19527,7 @@
       <c r="CM170" s="2"/>
       <c r="CN170" s="2"/>
     </row>
-    <row r="171" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
       <c r="E171" s="2"/>
@@ -19622,7 +19619,7 @@
       <c r="CM171" s="2"/>
       <c r="CN171" s="2"/>
     </row>
-    <row r="172" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
@@ -19714,7 +19711,7 @@
       <c r="CM172" s="2"/>
       <c r="CN172" s="2"/>
     </row>
-    <row r="173" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C173" s="2"/>
       <c r="D173" s="2"/>
       <c r="E173" s="2"/>
@@ -19806,7 +19803,7 @@
       <c r="CM173" s="2"/>
       <c r="CN173" s="2"/>
     </row>
-    <row r="174" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
@@ -19898,7 +19895,7 @@
       <c r="CM174" s="2"/>
       <c r="CN174" s="2"/>
     </row>
-    <row r="175" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C175" s="2"/>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
@@ -19990,7 +19987,7 @@
       <c r="CM175" s="2"/>
       <c r="CN175" s="2"/>
     </row>
-    <row r="176" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
@@ -20082,7 +20079,7 @@
       <c r="CM176" s="2"/>
       <c r="CN176" s="2"/>
     </row>
-    <row r="177" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="177" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C177" s="2"/>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
@@ -20174,7 +20171,7 @@
       <c r="CM177" s="2"/>
       <c r="CN177" s="2"/>
     </row>
-    <row r="178" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="178" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C178" s="2"/>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
@@ -20266,7 +20263,7 @@
       <c r="CM178" s="2"/>
       <c r="CN178" s="2"/>
     </row>
-    <row r="179" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="179" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C179" s="2"/>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
@@ -20358,7 +20355,7 @@
       <c r="CM179" s="2"/>
       <c r="CN179" s="2"/>
     </row>
-    <row r="180" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="180" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C180" s="2"/>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
@@ -20450,7 +20447,7 @@
       <c r="CM180" s="2"/>
       <c r="CN180" s="2"/>
     </row>
-    <row r="181" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="181" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C181" s="2"/>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
@@ -20542,7 +20539,7 @@
       <c r="CM181" s="2"/>
       <c r="CN181" s="2"/>
     </row>
-    <row r="182" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="182" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
@@ -20634,7 +20631,7 @@
       <c r="CM182" s="2"/>
       <c r="CN182" s="2"/>
     </row>
-    <row r="183" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="183" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
@@ -20726,7 +20723,7 @@
       <c r="CM183" s="2"/>
       <c r="CN183" s="2"/>
     </row>
-    <row r="184" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="184" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C184" s="2"/>
       <c r="D184" s="2"/>
       <c r="E184" s="2"/>
@@ -20818,7 +20815,7 @@
       <c r="CM184" s="2"/>
       <c r="CN184" s="2"/>
     </row>
-    <row r="185" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="185" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C185" s="2"/>
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
@@ -20910,7 +20907,7 @@
       <c r="CM185" s="2"/>
       <c r="CN185" s="2"/>
     </row>
-    <row r="186" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="186" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C186" s="2"/>
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
@@ -21002,7 +20999,7 @@
       <c r="CM186" s="2"/>
       <c r="CN186" s="2"/>
     </row>
-    <row r="187" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="187" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C187" s="2"/>
       <c r="D187" s="2"/>
       <c r="E187" s="2"/>
@@ -21094,7 +21091,7 @@
       <c r="CM187" s="2"/>
       <c r="CN187" s="2"/>
     </row>
-    <row r="188" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="188" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
       <c r="E188" s="2"/>
@@ -21186,7 +21183,7 @@
       <c r="CM188" s="2"/>
       <c r="CN188" s="2"/>
     </row>
-    <row r="189" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="189" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
@@ -21278,7 +21275,7 @@
       <c r="CM189" s="2"/>
       <c r="CN189" s="2"/>
     </row>
-    <row r="190" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="190" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C190" s="2"/>
       <c r="D190" s="2"/>
       <c r="E190" s="2"/>
@@ -21370,7 +21367,7 @@
       <c r="CM190" s="2"/>
       <c r="CN190" s="2"/>
     </row>
-    <row r="191" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="191" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C191" s="2"/>
       <c r="D191" s="2"/>
       <c r="E191" s="2"/>
@@ -21462,7 +21459,7 @@
       <c r="CM191" s="2"/>
       <c r="CN191" s="2"/>
     </row>
-    <row r="192" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="192" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C192" s="2"/>
       <c r="D192" s="2"/>
       <c r="E192" s="2"/>
@@ -21554,7 +21551,7 @@
       <c r="CM192" s="2"/>
       <c r="CN192" s="2"/>
     </row>
-    <row r="193" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="193" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
       <c r="E193" s="2"/>
@@ -21646,7 +21643,7 @@
       <c r="CM193" s="2"/>
       <c r="CN193" s="2"/>
     </row>
-    <row r="194" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="194" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
@@ -21738,7 +21735,7 @@
       <c r="CM194" s="2"/>
       <c r="CN194" s="2"/>
     </row>
-    <row r="195" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="195" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C195" s="2"/>
       <c r="D195" s="2"/>
       <c r="E195" s="2"/>
@@ -21830,7 +21827,7 @@
       <c r="CM195" s="2"/>
       <c r="CN195" s="2"/>
     </row>
-    <row r="196" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="196" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C196" s="2"/>
       <c r="D196" s="2"/>
       <c r="E196" s="2"/>
@@ -21922,7 +21919,7 @@
       <c r="CM196" s="2"/>
       <c r="CN196" s="2"/>
     </row>
-    <row r="197" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="197" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C197" s="2"/>
       <c r="D197" s="2"/>
       <c r="E197" s="2"/>
@@ -22014,7 +22011,7 @@
       <c r="CM197" s="2"/>
       <c r="CN197" s="2"/>
     </row>
-    <row r="198" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="198" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C198" s="2"/>
       <c r="D198" s="2"/>
       <c r="E198" s="2"/>
@@ -22106,7 +22103,7 @@
       <c r="CM198" s="2"/>
       <c r="CN198" s="2"/>
     </row>
-    <row r="199" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="199" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C199" s="2"/>
       <c r="D199" s="2"/>
       <c r="E199" s="2"/>
@@ -22198,7 +22195,7 @@
       <c r="CM199" s="2"/>
       <c r="CN199" s="2"/>
     </row>
-    <row r="200" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="200" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C200" s="2"/>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
@@ -22290,7 +22287,7 @@
       <c r="CM200" s="2"/>
       <c r="CN200" s="2"/>
     </row>
-    <row r="201" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="201" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C201" s="2"/>
       <c r="D201" s="2"/>
       <c r="E201" s="2"/>
@@ -22382,7 +22379,7 @@
       <c r="CM201" s="2"/>
       <c r="CN201" s="2"/>
     </row>
-    <row r="202" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="202" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C202" s="2"/>
       <c r="D202" s="2"/>
       <c r="E202" s="2"/>
@@ -22474,7 +22471,7 @@
       <c r="CM202" s="2"/>
       <c r="CN202" s="2"/>
     </row>
-    <row r="203" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="203" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C203" s="2"/>
       <c r="D203" s="2"/>
       <c r="E203" s="2"/>
@@ -22566,7 +22563,7 @@
       <c r="CM203" s="2"/>
       <c r="CN203" s="2"/>
     </row>
-    <row r="204" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="204" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C204" s="2"/>
       <c r="D204" s="2"/>
       <c r="E204" s="2"/>
@@ -22658,7 +22655,7 @@
       <c r="CM204" s="2"/>
       <c r="CN204" s="2"/>
     </row>
-    <row r="205" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="205" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C205" s="2"/>
       <c r="D205" s="2"/>
       <c r="E205" s="2"/>
@@ -22750,7 +22747,7 @@
       <c r="CM205" s="2"/>
       <c r="CN205" s="2"/>
     </row>
-    <row r="206" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="206" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C206" s="2"/>
       <c r="D206" s="2"/>
       <c r="E206" s="2"/>
@@ -22842,7 +22839,7 @@
       <c r="CM206" s="2"/>
       <c r="CN206" s="2"/>
     </row>
-    <row r="207" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="207" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C207" s="2"/>
       <c r="D207" s="2"/>
       <c r="E207" s="2"/>
@@ -22934,7 +22931,7 @@
       <c r="CM207" s="2"/>
       <c r="CN207" s="2"/>
     </row>
-    <row r="208" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="208" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C208" s="2"/>
       <c r="D208" s="2"/>
       <c r="E208" s="2"/>
@@ -23026,7 +23023,7 @@
       <c r="CM208" s="2"/>
       <c r="CN208" s="2"/>
     </row>
-    <row r="209" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="209" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C209" s="2"/>
       <c r="D209" s="2"/>
       <c r="E209" s="2"/>
@@ -23118,7 +23115,7 @@
       <c r="CM209" s="2"/>
       <c r="CN209" s="2"/>
     </row>
-    <row r="210" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="210" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
       <c r="E210" s="2"/>
@@ -23210,7 +23207,7 @@
       <c r="CM210" s="2"/>
       <c r="CN210" s="2"/>
     </row>
-    <row r="211" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="211" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C211" s="2"/>
       <c r="D211" s="2"/>
       <c r="E211" s="2"/>
@@ -23302,7 +23299,7 @@
       <c r="CM211" s="2"/>
       <c r="CN211" s="2"/>
     </row>
-    <row r="212" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="212" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
       <c r="E212" s="2"/>
@@ -23394,7 +23391,7 @@
       <c r="CM212" s="2"/>
       <c r="CN212" s="2"/>
     </row>
-    <row r="213" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="213" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C213" s="2"/>
       <c r="D213" s="2"/>
       <c r="E213" s="2"/>
@@ -23486,7 +23483,7 @@
       <c r="CM213" s="2"/>
       <c r="CN213" s="2"/>
     </row>
-    <row r="214" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="214" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
       <c r="E214" s="2"/>
@@ -23578,7 +23575,7 @@
       <c r="CM214" s="2"/>
       <c r="CN214" s="2"/>
     </row>
-    <row r="215" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="215" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
       <c r="E215" s="2"/>
@@ -23670,7 +23667,7 @@
       <c r="CM215" s="2"/>
       <c r="CN215" s="2"/>
     </row>
-    <row r="216" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="216" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
       <c r="E216" s="2"/>
@@ -23762,7 +23759,7 @@
       <c r="CM216" s="2"/>
       <c r="CN216" s="2"/>
     </row>
-    <row r="217" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="217" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
       <c r="E217" s="2"/>
@@ -23854,7 +23851,7 @@
       <c r="CM217" s="2"/>
       <c r="CN217" s="2"/>
     </row>
-    <row r="218" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="218" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
       <c r="E218" s="2"/>
@@ -23946,7 +23943,7 @@
       <c r="CM218" s="2"/>
       <c r="CN218" s="2"/>
     </row>
-    <row r="219" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="219" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
       <c r="E219" s="2"/>
@@ -24038,7 +24035,7 @@
       <c r="CM219" s="2"/>
       <c r="CN219" s="2"/>
     </row>
-    <row r="220" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="220" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
       <c r="E220" s="2"/>
@@ -24130,7 +24127,7 @@
       <c r="CM220" s="2"/>
       <c r="CN220" s="2"/>
     </row>
-    <row r="221" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="221" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
@@ -24222,7 +24219,7 @@
       <c r="CM221" s="2"/>
       <c r="CN221" s="2"/>
     </row>
-    <row r="222" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="222" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
       <c r="E222" s="2"/>
@@ -24314,7 +24311,7 @@
       <c r="CM222" s="2"/>
       <c r="CN222" s="2"/>
     </row>
-    <row r="223" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="223" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C223" s="2"/>
       <c r="D223" s="2"/>
       <c r="E223" s="2"/>
@@ -24406,7 +24403,7 @@
       <c r="CM223" s="2"/>
       <c r="CN223" s="2"/>
     </row>
-    <row r="224" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="224" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
       <c r="E224" s="2"/>
@@ -24498,7 +24495,7 @@
       <c r="CM224" s="2"/>
       <c r="CN224" s="2"/>
     </row>
-    <row r="225" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="225" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C225" s="2"/>
       <c r="D225" s="2"/>
       <c r="E225" s="2"/>
@@ -24590,7 +24587,7 @@
       <c r="CM225" s="2"/>
       <c r="CN225" s="2"/>
     </row>
-    <row r="226" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="226" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C226" s="2"/>
       <c r="D226" s="2"/>
       <c r="E226" s="2"/>
@@ -24682,7 +24679,7 @@
       <c r="CM226" s="2"/>
       <c r="CN226" s="2"/>
     </row>
-    <row r="227" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="227" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C227" s="2"/>
       <c r="D227" s="2"/>
       <c r="E227" s="2"/>
@@ -24774,7 +24771,7 @@
       <c r="CM227" s="2"/>
       <c r="CN227" s="2"/>
     </row>
-    <row r="228" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="228" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C228" s="2"/>
       <c r="D228" s="2"/>
       <c r="E228" s="2"/>
@@ -24866,7 +24863,7 @@
       <c r="CM228" s="2"/>
       <c r="CN228" s="2"/>
     </row>
-    <row r="229" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="229" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
       <c r="E229" s="2"/>
@@ -24958,7 +24955,7 @@
       <c r="CM229" s="2"/>
       <c r="CN229" s="2"/>
     </row>
-    <row r="230" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="230" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C230" s="2"/>
       <c r="D230" s="2"/>
       <c r="E230" s="2"/>
@@ -25050,7 +25047,7 @@
       <c r="CM230" s="2"/>
       <c r="CN230" s="2"/>
     </row>
-    <row r="231" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="231" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C231" s="2"/>
       <c r="D231" s="2"/>
       <c r="E231" s="2"/>
@@ -25142,7 +25139,7 @@
       <c r="CM231" s="2"/>
       <c r="CN231" s="2"/>
     </row>
-    <row r="232" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="232" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C232" s="2"/>
       <c r="D232" s="2"/>
       <c r="E232" s="2"/>
@@ -25234,7 +25231,7 @@
       <c r="CM232" s="2"/>
       <c r="CN232" s="2"/>
     </row>
-    <row r="233" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="233" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C233" s="2"/>
       <c r="D233" s="2"/>
       <c r="E233" s="2"/>
@@ -25326,7 +25323,7 @@
       <c r="CM233" s="2"/>
       <c r="CN233" s="2"/>
     </row>
-    <row r="234" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="234" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C234" s="2"/>
       <c r="D234" s="2"/>
       <c r="E234" s="2"/>
@@ -25418,7 +25415,7 @@
       <c r="CM234" s="2"/>
       <c r="CN234" s="2"/>
     </row>
-    <row r="235" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="235" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C235" s="2"/>
       <c r="D235" s="2"/>
       <c r="E235" s="2"/>
@@ -25510,7 +25507,7 @@
       <c r="CM235" s="2"/>
       <c r="CN235" s="2"/>
     </row>
-    <row r="236" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="236" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C236" s="2"/>
       <c r="D236" s="2"/>
       <c r="E236" s="2"/>
@@ -25602,7 +25599,7 @@
       <c r="CM236" s="2"/>
       <c r="CN236" s="2"/>
     </row>
-    <row r="237" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="237" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C237" s="2"/>
       <c r="D237" s="2"/>
       <c r="E237" s="2"/>
@@ -25694,7 +25691,7 @@
       <c r="CM237" s="2"/>
       <c r="CN237" s="2"/>
     </row>
-    <row r="238" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="238" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C238" s="2"/>
       <c r="D238" s="2"/>
       <c r="E238" s="2"/>
@@ -25786,7 +25783,7 @@
       <c r="CM238" s="2"/>
       <c r="CN238" s="2"/>
     </row>
-    <row r="239" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="239" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C239" s="2"/>
       <c r="D239" s="2"/>
       <c r="E239" s="2"/>
@@ -25878,7 +25875,7 @@
       <c r="CM239" s="2"/>
       <c r="CN239" s="2"/>
     </row>
-    <row r="240" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="240" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C240" s="2"/>
       <c r="D240" s="2"/>
       <c r="E240" s="2"/>
@@ -25970,7 +25967,7 @@
       <c r="CM240" s="2"/>
       <c r="CN240" s="2"/>
     </row>
-    <row r="241" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C241" s="2"/>
       <c r="D241" s="2"/>
       <c r="E241" s="2"/>
@@ -26062,7 +26059,7 @@
       <c r="CM241" s="2"/>
       <c r="CN241" s="2"/>
     </row>
-    <row r="242" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C242" s="2"/>
       <c r="D242" s="2"/>
       <c r="E242" s="2"/>
@@ -26154,7 +26151,7 @@
       <c r="CM242" s="2"/>
       <c r="CN242" s="2"/>
     </row>
-    <row r="243" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C243" s="2"/>
       <c r="D243" s="2"/>
       <c r="E243" s="2"/>
@@ -26246,7 +26243,7 @@
       <c r="CM243" s="2"/>
       <c r="CN243" s="2"/>
     </row>
-    <row r="244" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C244" s="2"/>
       <c r="D244" s="2"/>
       <c r="E244" s="2"/>
@@ -26338,7 +26335,7 @@
       <c r="CM244" s="2"/>
       <c r="CN244" s="2"/>
     </row>
-    <row r="245" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C245" s="2"/>
       <c r="D245" s="2"/>
       <c r="E245" s="2"/>
@@ -26430,7 +26427,7 @@
       <c r="CM245" s="2"/>
       <c r="CN245" s="2"/>
     </row>
-    <row r="246" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C246" s="2"/>
       <c r="D246" s="2"/>
       <c r="E246" s="2"/>
@@ -26522,7 +26519,7 @@
       <c r="CM246" s="2"/>
       <c r="CN246" s="2"/>
     </row>
-    <row r="247" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C247" s="2"/>
       <c r="D247" s="2"/>
       <c r="E247" s="2"/>
@@ -26614,7 +26611,7 @@
       <c r="CM247" s="2"/>
       <c r="CN247" s="2"/>
     </row>
-    <row r="248" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C248" s="2"/>
       <c r="D248" s="2"/>
       <c r="E248" s="2"/>
@@ -26706,7 +26703,7 @@
       <c r="CM248" s="2"/>
       <c r="CN248" s="2"/>
     </row>
-    <row r="249" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C249" s="2"/>
       <c r="D249" s="2"/>
       <c r="E249" s="2"/>
@@ -26798,7 +26795,7 @@
       <c r="CM249" s="2"/>
       <c r="CN249" s="2"/>
     </row>
-    <row r="250" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C250" s="2"/>
       <c r="D250" s="2"/>
       <c r="E250" s="2"/>
@@ -26890,7 +26887,7 @@
       <c r="CM250" s="2"/>
       <c r="CN250" s="2"/>
     </row>
-    <row r="251" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C251" s="2"/>
       <c r="D251" s="2"/>
       <c r="E251" s="2"/>
@@ -26982,7 +26979,7 @@
       <c r="CM251" s="2"/>
       <c r="CN251" s="2"/>
     </row>
-    <row r="252" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C252" s="2"/>
       <c r="D252" s="2"/>
       <c r="E252" s="2"/>
@@ -27074,7 +27071,7 @@
       <c r="CM252" s="2"/>
       <c r="CN252" s="2"/>
     </row>
-    <row r="253" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="253" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C253" s="2"/>
       <c r="D253" s="2"/>
       <c r="E253" s="2"/>
@@ -27166,7 +27163,7 @@
       <c r="CM253" s="2"/>
       <c r="CN253" s="2"/>
     </row>
-    <row r="254" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C254" s="2"/>
       <c r="D254" s="2"/>
       <c r="E254" s="2"/>
@@ -27258,7 +27255,7 @@
       <c r="CM254" s="2"/>
       <c r="CN254" s="2"/>
     </row>
-    <row r="255" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C255" s="2"/>
       <c r="D255" s="2"/>
       <c r="E255" s="2"/>
@@ -27350,7 +27347,7 @@
       <c r="CM255" s="2"/>
       <c r="CN255" s="2"/>
     </row>
-    <row r="256" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C256" s="2"/>
       <c r="D256" s="2"/>
       <c r="E256" s="2"/>
@@ -27442,7 +27439,7 @@
       <c r="CM256" s="2"/>
       <c r="CN256" s="2"/>
     </row>
-    <row r="257" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C257" s="2"/>
       <c r="D257" s="2"/>
       <c r="E257" s="2"/>
@@ -27534,7 +27531,7 @@
       <c r="CM257" s="2"/>
       <c r="CN257" s="2"/>
     </row>
-    <row r="258" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C258" s="2"/>
       <c r="D258" s="2"/>
       <c r="E258" s="2"/>
@@ -27626,7 +27623,7 @@
       <c r="CM258" s="2"/>
       <c r="CN258" s="2"/>
     </row>
-    <row r="259" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
       <c r="E259" s="2"/>
@@ -27718,7 +27715,7 @@
       <c r="CM259" s="2"/>
       <c r="CN259" s="2"/>
     </row>
-    <row r="260" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C260" s="2"/>
       <c r="D260" s="2"/>
       <c r="E260" s="2"/>
@@ -27810,7 +27807,7 @@
       <c r="CM260" s="2"/>
       <c r="CN260" s="2"/>
     </row>
-    <row r="261" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
       <c r="E261" s="2"/>
@@ -27902,7 +27899,7 @@
       <c r="CM261" s="2"/>
       <c r="CN261" s="2"/>
     </row>
-    <row r="262" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
       <c r="E262" s="2"/>
@@ -27994,7 +27991,7 @@
       <c r="CM262" s="2"/>
       <c r="CN262" s="2"/>
     </row>
-    <row r="263" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C263" s="2"/>
       <c r="D263" s="2"/>
       <c r="E263" s="2"/>
@@ -28086,7 +28083,7 @@
       <c r="CM263" s="2"/>
       <c r="CN263" s="2"/>
     </row>
-    <row r="264" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C264" s="2"/>
       <c r="D264" s="2"/>
       <c r="E264" s="2"/>
@@ -28178,7 +28175,7 @@
       <c r="CM264" s="2"/>
       <c r="CN264" s="2"/>
     </row>
-    <row r="265" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C265" s="2"/>
       <c r="D265" s="2"/>
       <c r="E265" s="2"/>
@@ -28270,7 +28267,7 @@
       <c r="CM265" s="2"/>
       <c r="CN265" s="2"/>
     </row>
-    <row r="266" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C266" s="2"/>
       <c r="D266" s="2"/>
       <c r="E266" s="2"/>
@@ -28362,7 +28359,7 @@
       <c r="CM266" s="2"/>
       <c r="CN266" s="2"/>
     </row>
-    <row r="267" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C267" s="2"/>
       <c r="D267" s="2"/>
       <c r="E267" s="2"/>
@@ -28454,7 +28451,7 @@
       <c r="CM267" s="2"/>
       <c r="CN267" s="2"/>
     </row>
-    <row r="268" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C268" s="2"/>
       <c r="D268" s="2"/>
       <c r="E268" s="2"/>
@@ -28546,7 +28543,7 @@
       <c r="CM268" s="2"/>
       <c r="CN268" s="2"/>
     </row>
-    <row r="269" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C269" s="2"/>
       <c r="D269" s="2"/>
       <c r="E269" s="2"/>
@@ -28638,7 +28635,7 @@
       <c r="CM269" s="2"/>
       <c r="CN269" s="2"/>
     </row>
-    <row r="270" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C270" s="2"/>
       <c r="D270" s="2"/>
       <c r="E270" s="2"/>
@@ -28730,7 +28727,7 @@
       <c r="CM270" s="2"/>
       <c r="CN270" s="2"/>
     </row>
-    <row r="271" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C271" s="2"/>
       <c r="D271" s="2"/>
       <c r="E271" s="2"/>
@@ -28822,7 +28819,7 @@
       <c r="CM271" s="2"/>
       <c r="CN271" s="2"/>
     </row>
-    <row r="272" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C272" s="2"/>
       <c r="D272" s="2"/>
       <c r="E272" s="2"/>
@@ -28914,7 +28911,7 @@
       <c r="CM272" s="2"/>
       <c r="CN272" s="2"/>
     </row>
-    <row r="273" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C273" s="2"/>
       <c r="D273" s="2"/>
       <c r="E273" s="2"/>
@@ -29006,7 +29003,7 @@
       <c r="CM273" s="2"/>
       <c r="CN273" s="2"/>
     </row>
-    <row r="274" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C274" s="2"/>
       <c r="D274" s="2"/>
       <c r="E274" s="2"/>
@@ -29098,7 +29095,7 @@
       <c r="CM274" s="2"/>
       <c r="CN274" s="2"/>
     </row>
-    <row r="275" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C275" s="2"/>
       <c r="D275" s="2"/>
       <c r="E275" s="2"/>
@@ -29190,7 +29187,7 @@
       <c r="CM275" s="2"/>
       <c r="CN275" s="2"/>
     </row>
-    <row r="276" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C276" s="2"/>
       <c r="D276" s="2"/>
       <c r="E276" s="2"/>
@@ -29282,7 +29279,7 @@
       <c r="CM276" s="2"/>
       <c r="CN276" s="2"/>
     </row>
-    <row r="277" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C277" s="2"/>
       <c r="D277" s="2"/>
       <c r="E277" s="2"/>
@@ -29374,7 +29371,7 @@
       <c r="CM277" s="2"/>
       <c r="CN277" s="2"/>
     </row>
-    <row r="278" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C278" s="2"/>
       <c r="D278" s="2"/>
       <c r="E278" s="2"/>
@@ -29466,7 +29463,7 @@
       <c r="CM278" s="2"/>
       <c r="CN278" s="2"/>
     </row>
-    <row r="279" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C279" s="2"/>
       <c r="D279" s="2"/>
       <c r="E279" s="2"/>
@@ -29558,7 +29555,7 @@
       <c r="CM279" s="2"/>
       <c r="CN279" s="2"/>
     </row>
-    <row r="280" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C280" s="2"/>
       <c r="D280" s="2"/>
       <c r="E280" s="2"/>
@@ -29650,7 +29647,7 @@
       <c r="CM280" s="2"/>
       <c r="CN280" s="2"/>
     </row>
-    <row r="281" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C281" s="2"/>
       <c r="D281" s="2"/>
       <c r="E281" s="2"/>
@@ -29742,7 +29739,7 @@
       <c r="CM281" s="2"/>
       <c r="CN281" s="2"/>
     </row>
-    <row r="282" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C282" s="2"/>
       <c r="D282" s="2"/>
       <c r="E282" s="2"/>
@@ -29834,7 +29831,7 @@
       <c r="CM282" s="2"/>
       <c r="CN282" s="2"/>
     </row>
-    <row r="283" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C283" s="2"/>
       <c r="D283" s="2"/>
       <c r="E283" s="2"/>
@@ -29926,7 +29923,7 @@
       <c r="CM283" s="2"/>
       <c r="CN283" s="2"/>
     </row>
-    <row r="284" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C284" s="2"/>
       <c r="D284" s="2"/>
       <c r="E284" s="2"/>
@@ -30018,7 +30015,7 @@
       <c r="CM284" s="2"/>
       <c r="CN284" s="2"/>
     </row>
-    <row r="285" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C285" s="2"/>
       <c r="D285" s="2"/>
       <c r="E285" s="2"/>
@@ -30110,7 +30107,7 @@
       <c r="CM285" s="2"/>
       <c r="CN285" s="2"/>
     </row>
-    <row r="286" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C286" s="2"/>
       <c r="D286" s="2"/>
       <c r="E286" s="2"/>
@@ -30202,7 +30199,7 @@
       <c r="CM286" s="2"/>
       <c r="CN286" s="2"/>
     </row>
-    <row r="287" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C287" s="2"/>
       <c r="D287" s="2"/>
       <c r="E287" s="2"/>
@@ -30294,7 +30291,7 @@
       <c r="CM287" s="2"/>
       <c r="CN287" s="2"/>
     </row>
-    <row r="288" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C288" s="2"/>
       <c r="D288" s="2"/>
       <c r="E288" s="2"/>
@@ -30386,7 +30383,7 @@
       <c r="CM288" s="2"/>
       <c r="CN288" s="2"/>
     </row>
-    <row r="289" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="289" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C289" s="2"/>
       <c r="D289" s="2"/>
       <c r="E289" s="2"/>
@@ -30478,7 +30475,7 @@
       <c r="CM289" s="2"/>
       <c r="CN289" s="2"/>
     </row>
-    <row r="290" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="290" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C290" s="2"/>
       <c r="D290" s="2"/>
       <c r="E290" s="2"/>
@@ -30570,7 +30567,7 @@
       <c r="CM290" s="2"/>
       <c r="CN290" s="2"/>
     </row>
-    <row r="291" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="291" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C291" s="2"/>
       <c r="D291" s="2"/>
       <c r="E291" s="2"/>
@@ -30662,7 +30659,7 @@
       <c r="CM291" s="2"/>
       <c r="CN291" s="2"/>
     </row>
-    <row r="292" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="292" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C292" s="2"/>
       <c r="D292" s="2"/>
       <c r="E292" s="2"/>
@@ -30754,7 +30751,7 @@
       <c r="CM292" s="2"/>
       <c r="CN292" s="2"/>
     </row>
-    <row r="293" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="293" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C293" s="2"/>
       <c r="D293" s="2"/>
       <c r="E293" s="2"/>
@@ -30846,7 +30843,7 @@
       <c r="CM293" s="2"/>
       <c r="CN293" s="2"/>
     </row>
-    <row r="294" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="294" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C294" s="2"/>
       <c r="D294" s="2"/>
       <c r="E294" s="2"/>
@@ -30938,7 +30935,7 @@
       <c r="CM294" s="2"/>
       <c r="CN294" s="2"/>
     </row>
-    <row r="295" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="295" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C295" s="2"/>
       <c r="D295" s="2"/>
       <c r="E295" s="2"/>
@@ -31030,7 +31027,7 @@
       <c r="CM295" s="2"/>
       <c r="CN295" s="2"/>
     </row>
-    <row r="296" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="296" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C296" s="2"/>
       <c r="D296" s="2"/>
       <c r="E296" s="2"/>
@@ -31122,7 +31119,7 @@
       <c r="CM296" s="2"/>
       <c r="CN296" s="2"/>
     </row>
-    <row r="297" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="297" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C297" s="2"/>
       <c r="D297" s="2"/>
       <c r="E297" s="2"/>
@@ -31214,7 +31211,7 @@
       <c r="CM297" s="2"/>
       <c r="CN297" s="2"/>
     </row>
-    <row r="298" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="298" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C298" s="2"/>
       <c r="D298" s="2"/>
       <c r="E298" s="2"/>
@@ -31306,7 +31303,7 @@
       <c r="CM298" s="2"/>
       <c r="CN298" s="2"/>
     </row>
-    <row r="299" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="299" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C299" s="2"/>
       <c r="D299" s="2"/>
       <c r="E299" s="2"/>
@@ -31398,7 +31395,7 @@
       <c r="CM299" s="2"/>
       <c r="CN299" s="2"/>
     </row>
-    <row r="300" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="300" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C300" s="2"/>
       <c r="D300" s="2"/>
       <c r="E300" s="2"/>
@@ -31490,7 +31487,7 @@
       <c r="CM300" s="2"/>
       <c r="CN300" s="2"/>
     </row>
-    <row r="301" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="301" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C301" s="2"/>
       <c r="D301" s="2"/>
       <c r="E301" s="2"/>
@@ -31582,7 +31579,7 @@
       <c r="CM301" s="2"/>
       <c r="CN301" s="2"/>
     </row>
-    <row r="302" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="302" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C302" s="2"/>
       <c r="D302" s="2"/>
       <c r="E302" s="2"/>
@@ -31674,7 +31671,7 @@
       <c r="CM302" s="2"/>
       <c r="CN302" s="2"/>
     </row>
-    <row r="303" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="303" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C303" s="2"/>
       <c r="D303" s="2"/>
       <c r="E303" s="2"/>
@@ -31766,7 +31763,7 @@
       <c r="CM303" s="2"/>
       <c r="CN303" s="2"/>
     </row>
-    <row r="304" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="304" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C304" s="2"/>
       <c r="D304" s="2"/>
       <c r="E304" s="2"/>
@@ -31858,7 +31855,7 @@
       <c r="CM304" s="2"/>
       <c r="CN304" s="2"/>
     </row>
-    <row r="305" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="305" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C305" s="2"/>
       <c r="D305" s="2"/>
       <c r="E305" s="2"/>
@@ -31950,7 +31947,7 @@
       <c r="CM305" s="2"/>
       <c r="CN305" s="2"/>
     </row>
-    <row r="306" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="306" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C306" s="2"/>
       <c r="D306" s="2"/>
       <c r="E306" s="2"/>
@@ -32042,7 +32039,7 @@
       <c r="CM306" s="2"/>
       <c r="CN306" s="2"/>
     </row>
-    <row r="307" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="307" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C307" s="2"/>
       <c r="D307" s="2"/>
       <c r="E307" s="2"/>
@@ -32134,7 +32131,7 @@
       <c r="CM307" s="2"/>
       <c r="CN307" s="2"/>
     </row>
-    <row r="308" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="308" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C308" s="2"/>
       <c r="D308" s="2"/>
       <c r="E308" s="2"/>
@@ -32226,7 +32223,7 @@
       <c r="CM308" s="2"/>
       <c r="CN308" s="2"/>
     </row>
-    <row r="309" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="309" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C309" s="2"/>
       <c r="D309" s="2"/>
       <c r="E309" s="2"/>
@@ -32318,7 +32315,7 @@
       <c r="CM309" s="2"/>
       <c r="CN309" s="2"/>
     </row>
-    <row r="310" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="310" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C310" s="2"/>
       <c r="D310" s="2"/>
       <c r="E310" s="2"/>
@@ -32410,7 +32407,7 @@
       <c r="CM310" s="2"/>
       <c r="CN310" s="2"/>
     </row>
-    <row r="311" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="311" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C311" s="2"/>
       <c r="D311" s="2"/>
       <c r="E311" s="2"/>
@@ -32502,7 +32499,7 @@
       <c r="CM311" s="2"/>
       <c r="CN311" s="2"/>
     </row>
-    <row r="312" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="312" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C312" s="2"/>
       <c r="D312" s="2"/>
       <c r="E312" s="2"/>
@@ -32594,7 +32591,7 @@
       <c r="CM312" s="2"/>
       <c r="CN312" s="2"/>
     </row>
-    <row r="313" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="313" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C313" s="2"/>
       <c r="D313" s="2"/>
       <c r="E313" s="2"/>
@@ -32686,7 +32683,7 @@
       <c r="CM313" s="2"/>
       <c r="CN313" s="2"/>
     </row>
-    <row r="314" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="314" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C314" s="2"/>
       <c r="D314" s="2"/>
       <c r="E314" s="2"/>
@@ -32778,7 +32775,7 @@
       <c r="CM314" s="2"/>
       <c r="CN314" s="2"/>
     </row>
-    <row r="315" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="315" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C315" s="2"/>
       <c r="D315" s="2"/>
       <c r="E315" s="2"/>
@@ -32870,7 +32867,7 @@
       <c r="CM315" s="2"/>
       <c r="CN315" s="2"/>
     </row>
-    <row r="316" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="316" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C316" s="2"/>
       <c r="D316" s="2"/>
       <c r="E316" s="2"/>
@@ -32962,7 +32959,7 @@
       <c r="CM316" s="2"/>
       <c r="CN316" s="2"/>
     </row>
-    <row r="317" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="317" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C317" s="2"/>
       <c r="D317" s="2"/>
       <c r="E317" s="2"/>
@@ -33054,7 +33051,7 @@
       <c r="CM317" s="2"/>
       <c r="CN317" s="2"/>
     </row>
-    <row r="318" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="318" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C318" s="2"/>
       <c r="D318" s="2"/>
       <c r="E318" s="2"/>
@@ -33146,7 +33143,7 @@
       <c r="CM318" s="2"/>
       <c r="CN318" s="2"/>
     </row>
-    <row r="319" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="319" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C319" s="2"/>
       <c r="D319" s="2"/>
       <c r="E319" s="2"/>
@@ -33238,7 +33235,7 @@
       <c r="CM319" s="2"/>
       <c r="CN319" s="2"/>
     </row>
-    <row r="320" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="320" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C320" s="2"/>
       <c r="D320" s="2"/>
       <c r="E320" s="2"/>
@@ -33330,7 +33327,7 @@
       <c r="CM320" s="2"/>
       <c r="CN320" s="2"/>
     </row>
-    <row r="321" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="321" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C321" s="2"/>
       <c r="D321" s="2"/>
       <c r="E321" s="2"/>
@@ -33422,7 +33419,7 @@
       <c r="CM321" s="2"/>
       <c r="CN321" s="2"/>
     </row>
-    <row r="322" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="322" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C322" s="2"/>
       <c r="D322" s="2"/>
       <c r="E322" s="2"/>
@@ -33514,7 +33511,7 @@
       <c r="CM322" s="2"/>
       <c r="CN322" s="2"/>
     </row>
-    <row r="323" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="323" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C323" s="2"/>
       <c r="D323" s="2"/>
       <c r="E323" s="2"/>
@@ -33606,7 +33603,7 @@
       <c r="CM323" s="2"/>
       <c r="CN323" s="2"/>
     </row>
-    <row r="324" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="324" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C324" s="2"/>
       <c r="D324" s="2"/>
       <c r="E324" s="2"/>
@@ -33698,7 +33695,7 @@
       <c r="CM324" s="2"/>
       <c r="CN324" s="2"/>
     </row>
-    <row r="325" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="325" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C325" s="2"/>
       <c r="D325" s="2"/>
       <c r="E325" s="2"/>
@@ -33790,7 +33787,7 @@
       <c r="CM325" s="2"/>
       <c r="CN325" s="2"/>
     </row>
-    <row r="326" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="326" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C326" s="2"/>
       <c r="D326" s="2"/>
       <c r="E326" s="2"/>
@@ -33882,7 +33879,7 @@
       <c r="CM326" s="2"/>
       <c r="CN326" s="2"/>
     </row>
-    <row r="327" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="327" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C327" s="2"/>
       <c r="D327" s="2"/>
       <c r="E327" s="2"/>
@@ -33974,7 +33971,7 @@
       <c r="CM327" s="2"/>
       <c r="CN327" s="2"/>
     </row>
-    <row r="328" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="328" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C328" s="2"/>
       <c r="D328" s="2"/>
       <c r="E328" s="2"/>
@@ -34066,7 +34063,7 @@
       <c r="CM328" s="2"/>
       <c r="CN328" s="2"/>
     </row>
-    <row r="329" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="329" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C329" s="2"/>
       <c r="D329" s="2"/>
       <c r="E329" s="2"/>
@@ -34158,7 +34155,7 @@
       <c r="CM329" s="2"/>
       <c r="CN329" s="2"/>
     </row>
-    <row r="330" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="330" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C330" s="2"/>
       <c r="D330" s="2"/>
       <c r="E330" s="2"/>
@@ -34250,7 +34247,7 @@
       <c r="CM330" s="2"/>
       <c r="CN330" s="2"/>
     </row>
-    <row r="331" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="331" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C331" s="2"/>
       <c r="D331" s="2"/>
       <c r="E331" s="2"/>
@@ -34342,7 +34339,7 @@
       <c r="CM331" s="2"/>
       <c r="CN331" s="2"/>
     </row>
-    <row r="332" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="332" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C332" s="2"/>
       <c r="D332" s="2"/>
       <c r="E332" s="2"/>
@@ -34434,7 +34431,7 @@
       <c r="CM332" s="2"/>
       <c r="CN332" s="2"/>
     </row>
-    <row r="333" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="333" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C333" s="2"/>
       <c r="D333" s="2"/>
       <c r="E333" s="2"/>
@@ -34526,7 +34523,7 @@
       <c r="CM333" s="2"/>
       <c r="CN333" s="2"/>
     </row>
-    <row r="334" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="334" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C334" s="2"/>
       <c r="D334" s="2"/>
       <c r="E334" s="2"/>
@@ -34618,7 +34615,7 @@
       <c r="CM334" s="2"/>
       <c r="CN334" s="2"/>
     </row>
-    <row r="335" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="335" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C335" s="2"/>
       <c r="D335" s="2"/>
       <c r="E335" s="2"/>
@@ -34710,7 +34707,7 @@
       <c r="CM335" s="2"/>
       <c r="CN335" s="2"/>
     </row>
-    <row r="336" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="336" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C336" s="2"/>
       <c r="D336" s="2"/>
       <c r="E336" s="2"/>
@@ -34802,7 +34799,7 @@
       <c r="CM336" s="2"/>
       <c r="CN336" s="2"/>
     </row>
-    <row r="337" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="337" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C337" s="2"/>
       <c r="D337" s="2"/>
       <c r="E337" s="2"/>
@@ -34894,7 +34891,7 @@
       <c r="CM337" s="2"/>
       <c r="CN337" s="2"/>
     </row>
-    <row r="338" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="338" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C338" s="2"/>
       <c r="D338" s="2"/>
       <c r="E338" s="2"/>
@@ -34986,7 +34983,7 @@
       <c r="CM338" s="2"/>
       <c r="CN338" s="2"/>
     </row>
-    <row r="339" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="339" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C339" s="2"/>
       <c r="D339" s="2"/>
       <c r="E339" s="2"/>
@@ -35078,7 +35075,7 @@
       <c r="CM339" s="2"/>
       <c r="CN339" s="2"/>
     </row>
-    <row r="340" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="340" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C340" s="2"/>
       <c r="D340" s="2"/>
       <c r="E340" s="2"/>
@@ -35170,7 +35167,7 @@
       <c r="CM340" s="2"/>
       <c r="CN340" s="2"/>
     </row>
-    <row r="341" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="341" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C341" s="2"/>
       <c r="D341" s="2"/>
       <c r="E341" s="2"/>
@@ -35262,7 +35259,7 @@
       <c r="CM341" s="2"/>
       <c r="CN341" s="2"/>
     </row>
-    <row r="342" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="342" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C342" s="2"/>
       <c r="D342" s="2"/>
       <c r="E342" s="2"/>
@@ -35354,7 +35351,7 @@
       <c r="CM342" s="2"/>
       <c r="CN342" s="2"/>
     </row>
-    <row r="343" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="343" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C343" s="2"/>
       <c r="D343" s="2"/>
       <c r="E343" s="2"/>
@@ -35446,7 +35443,7 @@
       <c r="CM343" s="2"/>
       <c r="CN343" s="2"/>
     </row>
-    <row r="344" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="344" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C344" s="2"/>
       <c r="D344" s="2"/>
       <c r="E344" s="2"/>
@@ -35538,7 +35535,7 @@
       <c r="CM344" s="2"/>
       <c r="CN344" s="2"/>
     </row>
-    <row r="345" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="345" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C345" s="2"/>
       <c r="D345" s="2"/>
       <c r="E345" s="2"/>
@@ -35630,7 +35627,7 @@
       <c r="CM345" s="2"/>
       <c r="CN345" s="2"/>
     </row>
-    <row r="346" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="346" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C346" s="2"/>
       <c r="D346" s="2"/>
       <c r="E346" s="2"/>
@@ -35722,7 +35719,7 @@
       <c r="CM346" s="2"/>
       <c r="CN346" s="2"/>
     </row>
-    <row r="347" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="347" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C347" s="2"/>
       <c r="D347" s="2"/>
       <c r="E347" s="2"/>
@@ -35814,7 +35811,7 @@
       <c r="CM347" s="2"/>
       <c r="CN347" s="2"/>
     </row>
-    <row r="348" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="348" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C348" s="2"/>
       <c r="D348" s="2"/>
       <c r="E348" s="2"/>
@@ -35906,7 +35903,7 @@
       <c r="CM348" s="2"/>
       <c r="CN348" s="2"/>
     </row>
-    <row r="349" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="349" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C349" s="2"/>
       <c r="D349" s="2"/>
       <c r="E349" s="2"/>
@@ -35998,7 +35995,7 @@
       <c r="CM349" s="2"/>
       <c r="CN349" s="2"/>
     </row>
-    <row r="350" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="350" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C350" s="2"/>
       <c r="D350" s="2"/>
       <c r="E350" s="2"/>
@@ -36090,7 +36087,7 @@
       <c r="CM350" s="2"/>
       <c r="CN350" s="2"/>
     </row>
-    <row r="351" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="351" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C351" s="2"/>
       <c r="D351" s="2"/>
       <c r="E351" s="2"/>
@@ -36182,7 +36179,7 @@
       <c r="CM351" s="2"/>
       <c r="CN351" s="2"/>
     </row>
-    <row r="352" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="352" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C352" s="2"/>
       <c r="D352" s="2"/>
       <c r="E352" s="2"/>
@@ -36274,7 +36271,7 @@
       <c r="CM352" s="2"/>
       <c r="CN352" s="2"/>
     </row>
-    <row r="353" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="353" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C353" s="2"/>
       <c r="D353" s="2"/>
       <c r="E353" s="2"/>
@@ -36366,7 +36363,7 @@
       <c r="CM353" s="2"/>
       <c r="CN353" s="2"/>
     </row>
-    <row r="354" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="354" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C354" s="2"/>
       <c r="D354" s="2"/>
       <c r="E354" s="2"/>
@@ -36458,7 +36455,7 @@
       <c r="CM354" s="2"/>
       <c r="CN354" s="2"/>
     </row>
-    <row r="355" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="355" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C355" s="2"/>
       <c r="D355" s="2"/>
       <c r="E355" s="2"/>
@@ -36550,7 +36547,7 @@
       <c r="CM355" s="2"/>
       <c r="CN355" s="2"/>
     </row>
-    <row r="356" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="356" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C356" s="2"/>
       <c r="D356" s="2"/>
       <c r="E356" s="2"/>
@@ -36642,7 +36639,7 @@
       <c r="CM356" s="2"/>
       <c r="CN356" s="2"/>
     </row>
-    <row r="357" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="357" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C357" s="2"/>
       <c r="D357" s="2"/>
       <c r="E357" s="2"/>
@@ -36734,7 +36731,7 @@
       <c r="CM357" s="2"/>
       <c r="CN357" s="2"/>
     </row>
-    <row r="358" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="358" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C358" s="2"/>
       <c r="D358" s="2"/>
       <c r="E358" s="2"/>
@@ -36826,7 +36823,7 @@
       <c r="CM358" s="2"/>
       <c r="CN358" s="2"/>
     </row>
-    <row r="359" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="359" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C359" s="2"/>
       <c r="D359" s="2"/>
       <c r="E359" s="2"/>
@@ -36918,7 +36915,7 @@
       <c r="CM359" s="2"/>
       <c r="CN359" s="2"/>
     </row>
-    <row r="360" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="360" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C360" s="2"/>
       <c r="D360" s="2"/>
       <c r="E360" s="2"/>
@@ -37010,7 +37007,7 @@
       <c r="CM360" s="2"/>
       <c r="CN360" s="2"/>
     </row>
-    <row r="361" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="361" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C361" s="2"/>
       <c r="D361" s="2"/>
       <c r="E361" s="2"/>
@@ -37102,7 +37099,7 @@
       <c r="CM361" s="2"/>
       <c r="CN361" s="2"/>
     </row>
-    <row r="362" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="362" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C362" s="2"/>
       <c r="D362" s="2"/>
       <c r="E362" s="2"/>
@@ -37194,7 +37191,7 @@
       <c r="CM362" s="2"/>
       <c r="CN362" s="2"/>
     </row>
-    <row r="363" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="363" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C363" s="2"/>
       <c r="D363" s="2"/>
       <c r="E363" s="2"/>
@@ -37286,7 +37283,7 @@
       <c r="CM363" s="2"/>
       <c r="CN363" s="2"/>
     </row>
-    <row r="364" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="364" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C364" s="2"/>
       <c r="D364" s="2"/>
       <c r="E364" s="2"/>
@@ -37378,7 +37375,7 @@
       <c r="CM364" s="2"/>
       <c r="CN364" s="2"/>
     </row>
-    <row r="365" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="365" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C365" s="2"/>
       <c r="D365" s="2"/>
       <c r="E365" s="2"/>
@@ -37470,7 +37467,7 @@
       <c r="CM365" s="2"/>
       <c r="CN365" s="2"/>
     </row>
-    <row r="366" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="366" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C366" s="2"/>
       <c r="D366" s="2"/>
       <c r="E366" s="2"/>
@@ -37562,7 +37559,7 @@
       <c r="CM366" s="2"/>
       <c r="CN366" s="2"/>
     </row>
-    <row r="367" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="367" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C367" s="2"/>
       <c r="D367" s="2"/>
       <c r="E367" s="2"/>
@@ -37654,7 +37651,7 @@
       <c r="CM367" s="2"/>
       <c r="CN367" s="2"/>
     </row>
-    <row r="368" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="368" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C368" s="2"/>
       <c r="D368" s="2"/>
       <c r="E368" s="2"/>
@@ -37746,7 +37743,7 @@
       <c r="CM368" s="2"/>
       <c r="CN368" s="2"/>
     </row>
-    <row r="369" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="369" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C369" s="2"/>
       <c r="D369" s="2"/>
       <c r="E369" s="2"/>
@@ -37838,7 +37835,7 @@
       <c r="CM369" s="2"/>
       <c r="CN369" s="2"/>
     </row>
-    <row r="370" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="370" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C370" s="2"/>
       <c r="D370" s="2"/>
       <c r="E370" s="2"/>
@@ -37930,7 +37927,7 @@
       <c r="CM370" s="2"/>
       <c r="CN370" s="2"/>
     </row>
-    <row r="371" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="371" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C371" s="2"/>
       <c r="D371" s="2"/>
       <c r="E371" s="2"/>
@@ -38022,7 +38019,7 @@
       <c r="CM371" s="2"/>
       <c r="CN371" s="2"/>
     </row>
-    <row r="372" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="372" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C372" s="2"/>
       <c r="D372" s="2"/>
       <c r="E372" s="2"/>
@@ -38114,7 +38111,7 @@
       <c r="CM372" s="2"/>
       <c r="CN372" s="2"/>
     </row>
-    <row r="373" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="373" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C373" s="2"/>
       <c r="D373" s="2"/>
       <c r="E373" s="2"/>
@@ -38206,7 +38203,7 @@
       <c r="CM373" s="2"/>
       <c r="CN373" s="2"/>
     </row>
-    <row r="374" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="374" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C374" s="2"/>
       <c r="D374" s="2"/>
       <c r="E374" s="2"/>
@@ -38298,7 +38295,7 @@
       <c r="CM374" s="2"/>
       <c r="CN374" s="2"/>
     </row>
-    <row r="375" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="375" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C375" s="2"/>
       <c r="D375" s="2"/>
       <c r="E375" s="2"/>
@@ -38390,7 +38387,7 @@
       <c r="CM375" s="2"/>
       <c r="CN375" s="2"/>
     </row>
-    <row r="376" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="376" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C376" s="2"/>
       <c r="D376" s="2"/>
       <c r="E376" s="2"/>
@@ -38482,7 +38479,7 @@
       <c r="CM376" s="2"/>
       <c r="CN376" s="2"/>
     </row>
-    <row r="377" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="377" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C377" s="2"/>
       <c r="D377" s="2"/>
       <c r="E377" s="2"/>
@@ -38574,7 +38571,7 @@
       <c r="CM377" s="2"/>
       <c r="CN377" s="2"/>
     </row>
-    <row r="378" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="378" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C378" s="2"/>
       <c r="D378" s="2"/>
       <c r="E378" s="2"/>
@@ -38666,7 +38663,7 @@
       <c r="CM378" s="2"/>
       <c r="CN378" s="2"/>
     </row>
-    <row r="379" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="379" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C379" s="2"/>
       <c r="D379" s="2"/>
       <c r="E379" s="2"/>
@@ -38758,7 +38755,7 @@
       <c r="CM379" s="2"/>
       <c r="CN379" s="2"/>
     </row>
-    <row r="380" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="380" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C380" s="2"/>
       <c r="D380" s="2"/>
       <c r="E380" s="2"/>
@@ -38850,7 +38847,7 @@
       <c r="CM380" s="2"/>
       <c r="CN380" s="2"/>
     </row>
-    <row r="381" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="381" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C381" s="2"/>
       <c r="D381" s="2"/>
       <c r="E381" s="2"/>
@@ -38942,7 +38939,7 @@
       <c r="CM381" s="2"/>
       <c r="CN381" s="2"/>
     </row>
-    <row r="382" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="382" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C382" s="2"/>
       <c r="D382" s="2"/>
       <c r="E382" s="2"/>
@@ -39034,7 +39031,7 @@
       <c r="CM382" s="2"/>
       <c r="CN382" s="2"/>
     </row>
-    <row r="383" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="383" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C383" s="2"/>
       <c r="D383" s="2"/>
       <c r="E383" s="2"/>
@@ -39126,7 +39123,7 @@
       <c r="CM383" s="2"/>
       <c r="CN383" s="2"/>
     </row>
-    <row r="384" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="384" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C384" s="2"/>
       <c r="D384" s="2"/>
       <c r="E384" s="2"/>
@@ -39218,7 +39215,7 @@
       <c r="CM384" s="2"/>
       <c r="CN384" s="2"/>
     </row>
-    <row r="385" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="385" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C385" s="2"/>
       <c r="D385" s="2"/>
       <c r="E385" s="2"/>
@@ -39310,7 +39307,7 @@
       <c r="CM385" s="2"/>
       <c r="CN385" s="2"/>
     </row>
-    <row r="386" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="386" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C386" s="2"/>
       <c r="D386" s="2"/>
       <c r="E386" s="2"/>
@@ -39402,7 +39399,7 @@
       <c r="CM386" s="2"/>
       <c r="CN386" s="2"/>
     </row>
-    <row r="387" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="387" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C387" s="2"/>
       <c r="D387" s="2"/>
       <c r="E387" s="2"/>
@@ -39494,7 +39491,7 @@
       <c r="CM387" s="2"/>
       <c r="CN387" s="2"/>
     </row>
-    <row r="388" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="388" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C388" s="2"/>
       <c r="D388" s="2"/>
       <c r="E388" s="2"/>
@@ -39586,7 +39583,7 @@
       <c r="CM388" s="2"/>
       <c r="CN388" s="2"/>
     </row>
-    <row r="389" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="389" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C389" s="2"/>
       <c r="D389" s="2"/>
       <c r="E389" s="2"/>
@@ -39678,7 +39675,7 @@
       <c r="CM389" s="2"/>
       <c r="CN389" s="2"/>
     </row>
-    <row r="390" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="390" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C390" s="2"/>
       <c r="D390" s="2"/>
       <c r="E390" s="2"/>
@@ -39770,7 +39767,7 @@
       <c r="CM390" s="2"/>
       <c r="CN390" s="2"/>
     </row>
-    <row r="391" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="391" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C391" s="2"/>
       <c r="D391" s="2"/>
       <c r="E391" s="2"/>
@@ -39862,7 +39859,7 @@
       <c r="CM391" s="2"/>
       <c r="CN391" s="2"/>
     </row>
-    <row r="392" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="392" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C392" s="2"/>
       <c r="D392" s="2"/>
       <c r="E392" s="2"/>
@@ -39954,7 +39951,7 @@
       <c r="CM392" s="2"/>
       <c r="CN392" s="2"/>
     </row>
-    <row r="393" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="393" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C393" s="2"/>
       <c r="D393" s="2"/>
       <c r="E393" s="2"/>
@@ -40046,7 +40043,7 @@
       <c r="CM393" s="2"/>
       <c r="CN393" s="2"/>
     </row>
-    <row r="394" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="394" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C394" s="2"/>
       <c r="D394" s="2"/>
       <c r="E394" s="2"/>
@@ -40138,7 +40135,7 @@
       <c r="CM394" s="2"/>
       <c r="CN394" s="2"/>
     </row>
-    <row r="395" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="395" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C395" s="2"/>
       <c r="D395" s="2"/>
       <c r="E395" s="2"/>
@@ -40230,7 +40227,7 @@
       <c r="CM395" s="2"/>
       <c r="CN395" s="2"/>
     </row>
-    <row r="396" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="396" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C396" s="2"/>
       <c r="D396" s="2"/>
       <c r="E396" s="2"/>
@@ -40322,7 +40319,7 @@
       <c r="CM396" s="2"/>
       <c r="CN396" s="2"/>
     </row>
-    <row r="397" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="397" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C397" s="2"/>
       <c r="D397" s="2"/>
       <c r="E397" s="2"/>
@@ -40414,7 +40411,7 @@
       <c r="CM397" s="2"/>
       <c r="CN397" s="2"/>
     </row>
-    <row r="398" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="398" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C398" s="2"/>
       <c r="D398" s="2"/>
       <c r="E398" s="2"/>
@@ -40506,7 +40503,7 @@
       <c r="CM398" s="2"/>
       <c r="CN398" s="2"/>
     </row>
-    <row r="399" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="399" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C399" s="2"/>
       <c r="D399" s="2"/>
       <c r="E399" s="2"/>
@@ -40598,7 +40595,7 @@
       <c r="CM399" s="2"/>
       <c r="CN399" s="2"/>
     </row>
-    <row r="400" spans="3:92" x14ac:dyDescent="0.25">
+    <row r="400" spans="3:92" x14ac:dyDescent="0.35">
       <c r="C400" s="2"/>
       <c r="D400" s="2"/>
       <c r="E400" s="2"/>
@@ -40773,12 +40770,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="17d0a144-7218-432a-80c1-1473a2ac0f84" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -40958,17 +40954,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="17d0a144-7218-432a-80c1-1473a2ac0f84" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4F67E43-074E-4C0F-B170-E53BCA717C8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B51BD707-A63C-4C12-A5D3-024A5FAE9E8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="17d0a144-7218-432a-80c1-1473a2ac0f84"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -40992,17 +40997,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B51BD707-A63C-4C12-A5D3-024A5FAE9E8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4F67E43-074E-4C0F-B170-E53BCA717C8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="17d0a144-7218-432a-80c1-1473a2ac0f84"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
test: Settlement reports view standard scenario tests (#2567)
* update

* update

* update

* update

* update

* update
</commit_message>
<xml_diff>
--- a/source/databricks/calculation_engine/tests/features/given_a_wholesale_calculation/when_minimal_standard_scenario/Oracle - wholesale minimal standard scenario.xlsx
+++ b/source/databricks/calculation_engine/tests/features/given_a_wholesale_calculation/when_minimal_standard_scenario/Oracle - wholesale minimal standard scenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\opengeh-wholesale\source\databricks\calculation_engine\tests\features\given_a_wholesale_calculation\when_minimal_standard_scenario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB31EB3E-37E5-4FFB-A553-56A8B89A7846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BA4F13-65CA-4B59-A0F3-4C42D49BBF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{B26405EC-4681-4CC9-BF80-F87B3459AD72}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="51420" windowHeight="21100" xr2:uid="{B26405EC-4681-4CC9-BF80-F87B3459AD72}"/>
   </bookViews>
   <sheets>
     <sheet name="Hour1" sheetId="11" r:id="rId1"/>
@@ -362,9 +362,6 @@
     <t>Number</t>
   </si>
   <si>
-    <t>ga_brp_es</t>
-  </si>
-  <si>
     <t>E17</t>
   </si>
   <si>
@@ -471,6 +468,9 @@
   </si>
   <si>
     <t>nonprofiled_consumption</t>
+  </si>
+  <si>
+    <t>ga</t>
   </si>
 </sst>
 </file>
@@ -622,7 +622,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -664,28 +664,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -741,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -788,17 +766,11 @@
     <xf numFmtId="164" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -811,28 +783,28 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1422,8 +1394,8 @@
   </sheetPr>
   <dimension ref="A1:CN400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I84" sqref="I84:I87"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1469,7 +1441,7 @@
         <v>22</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>7</v>
@@ -1493,7 +1465,7 @@
         <v>75</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K1" s="14" t="s">
         <v>8</v>
@@ -1540,53 +1512,53 @@
         <v>17</v>
       </c>
       <c r="AG1" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="AH1" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH1" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="AI1" s="47"/>
-      <c r="AJ1" s="47"/>
-      <c r="AK1" s="47"/>
+      <c r="AI1" s="45"/>
+      <c r="AJ1" s="45"/>
+      <c r="AK1" s="45"/>
     </row>
     <row r="2" spans="1:92" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>86</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>87</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="43">
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="41">
         <f t="shared" ref="J2:J19" si="0">IF(C2="","",SUM(F2:I2))</f>
         <v>0</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L2" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="N2" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="O2" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="O2" s="10" t="s">
-        <v>91</v>
       </c>
       <c r="P2" s="29"/>
       <c r="Q2" s="29"/>
@@ -1598,19 +1570,19 @@
         <f>SUMIFS(TableDay1[TotalHour],TableDay1[settlement_method],"D01",TableDay1[resolution],"PT15M")</f>
         <v>0</v>
       </c>
-      <c r="U2" s="42">
+      <c r="U2" s="40">
         <f>SUMIFS(TableDay1[Quarter1],TableDay1[settlement_method],"D01",TableDay1[resolution],"PT15M")</f>
         <v>0</v>
       </c>
-      <c r="V2" s="42">
+      <c r="V2" s="40">
         <f>SUMIFS(TableDay1[Quarter2],TableDay1[settlement_method],"D01",TableDay1[resolution],"PT15M")</f>
         <v>0</v>
       </c>
-      <c r="W2" s="42">
+      <c r="W2" s="40">
         <f>SUMIFS(TableDay1[Quarter3],TableDay1[settlement_method],"D01",TableDay1[resolution],"PT15M")</f>
         <v>0</v>
       </c>
-      <c r="X2" s="42">
+      <c r="X2" s="40">
         <f>SUMIFS(TableDay1[Quarter4],TableDay1[settlement_method],"D01",TableDay1[resolution],"PT15M")</f>
         <v>0</v>
       </c>
@@ -1635,47 +1607,47 @@
         <v>E02</v>
       </c>
       <c r="AH2" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="AI2" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="AI2" s="24" t="s">
+      <c r="AJ2" s="27" t="s">
         <v>108</v>
-      </c>
-      <c r="AJ2" s="27" t="s">
-        <v>109</v>
       </c>
       <c r="AK2" s="2"/>
       <c r="AL2" s="2"/>
     </row>
     <row r="3" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C3" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="43">
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K3" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>98</v>
-      </c>
       <c r="N3" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P3" s="29"/>
       <c r="Q3" s="29"/>
@@ -1687,19 +1659,19 @@
         <f>SUMIFS(TableDay1[TotalHour],TableDay1[settlement_method],"E02",TableDay1[resolution],"PT15M")</f>
         <v>17.5</v>
       </c>
-      <c r="U3" s="42">
+      <c r="U3" s="40">
         <f>SUMIFS(TableDay1[Quarter1],TableDay1[settlement_method],"E02",TableDay1[resolution],"PT15M")</f>
         <v>2.5</v>
       </c>
-      <c r="V3" s="42">
+      <c r="V3" s="40">
         <f>SUMIFS(TableDay1[Quarter2],TableDay1[settlement_method],"E02",TableDay1[resolution],"PT15M")</f>
         <v>2.5</v>
       </c>
-      <c r="W3" s="42">
+      <c r="W3" s="40">
         <f>SUMIFS(TableDay1[Quarter3],TableDay1[settlement_method],"E02",TableDay1[resolution],"PT15M")</f>
         <v>2.5</v>
       </c>
-      <c r="X3" s="42">
+      <c r="X3" s="40">
         <f>SUMIFS(TableDay1[Quarter4],TableDay1[settlement_method],"E02",TableDay1[resolution],"PT15M")</f>
         <v>10</v>
       </c>
@@ -1737,34 +1709,34 @@
     </row>
     <row r="4" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C4" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>86</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>87</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
-      <c r="J4" s="43">
+      <c r="J4" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="M4" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>90</v>
       </c>
       <c r="N4" s="10"/>
       <c r="O4" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P4" s="29"/>
       <c r="Q4" s="29"/>
@@ -1776,19 +1748,19 @@
         <f>SUMIFS(TableDay1[TotalHour],TableDay1[type],"E18",TableDay1[resolution],"PT15M")</f>
         <v>0</v>
       </c>
-      <c r="U4" s="42">
+      <c r="U4" s="40">
         <f>SUMIFS(TableDay1[Quarter1],TableDay1[type],"E18",TableDay1[resolution],"PT15M")</f>
         <v>0</v>
       </c>
-      <c r="V4" s="42">
+      <c r="V4" s="40">
         <f>SUMIFS(TableDay1[Quarter2],TableDay1[type],"E18",TableDay1[resolution],"PT15M")</f>
         <v>0</v>
       </c>
-      <c r="W4" s="42">
+      <c r="W4" s="40">
         <f>SUMIFS(TableDay1[Quarter3],TableDay1[type],"E18",TableDay1[resolution],"PT15M")</f>
         <v>0</v>
       </c>
-      <c r="X4" s="42">
+      <c r="X4" s="40">
         <f>SUMIFS(TableDay1[Quarter4],TableDay1[type],"E18",TableDay1[resolution],"PT15M")</f>
         <v>0</v>
       </c>
@@ -1821,9 +1793,9 @@
       <c r="E5" s="11"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="43" t="str">
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -1832,7 +1804,7 @@
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P5" s="29"/>
       <c r="Q5" s="29"/>
@@ -1844,19 +1816,19 @@
         <f>SUMIFS(TableDay1[TotalHour],TableDay1[type],"E17",TableDay1[resolution],"PT15M")</f>
         <v>17.5</v>
       </c>
-      <c r="U5" s="42">
+      <c r="U5" s="40">
         <f>SUMIFS(TableDay1[Quarter1],TableDay1[type],"E17",TableDay1[resolution],"PT15M")</f>
         <v>2.5</v>
       </c>
-      <c r="V5" s="42">
+      <c r="V5" s="40">
         <f>SUMIFS(TableDay1[Quarter2],TableDay1[type],"E17",TableDay1[resolution],"PT15M")</f>
         <v>2.5</v>
       </c>
-      <c r="W5" s="42">
+      <c r="W5" s="40">
         <f>SUMIFS(TableDay1[Quarter3],TableDay1[type],"E17",TableDay1[resolution],"PT15M")</f>
         <v>2.5</v>
       </c>
-      <c r="X5" s="42">
+      <c r="X5" s="40">
         <f>SUMIFS(TableDay1[Quarter4],TableDay1[type],"E17",TableDay1[resolution],"PT15M")</f>
         <v>10</v>
       </c>
@@ -1885,13 +1857,13 @@
     </row>
     <row r="6" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C6" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6" s="12">
         <v>20</v>
@@ -1899,22 +1871,22 @@
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
-      <c r="J6" s="43">
+      <c r="J6" s="41">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N6" s="10"/>
       <c r="O6" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P6" s="29"/>
       <c r="Q6" s="29"/>
@@ -1950,13 +1922,13 @@
     </row>
     <row r="7" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C7" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F7" s="12">
         <v>2.5</v>
@@ -1964,28 +1936,28 @@
       <c r="G7" s="12">
         <v>2.5</v>
       </c>
-      <c r="H7" s="41">
+      <c r="H7" s="39">
         <v>2.5</v>
       </c>
-      <c r="I7" s="41">
+      <c r="I7" s="39">
         <v>10</v>
       </c>
-      <c r="J7" s="43">
+      <c r="J7" s="41">
         <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N7" s="10"/>
       <c r="O7" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P7" s="29"/>
       <c r="Q7" s="29"/>
@@ -2021,34 +1993,34 @@
     </row>
     <row r="8" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C8" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="12">
         <v>40.158999999999999</v>
       </c>
       <c r="G8" s="12"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="43">
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="41">
         <f t="shared" si="0"/>
         <v>40.158999999999999</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N8" s="10"/>
       <c r="O8" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P8" s="29"/>
       <c r="Q8" s="29"/>
@@ -2088,9 +2060,9 @@
       <c r="E9" s="11"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="43" t="str">
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2099,7 +2071,7 @@
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P9" s="29"/>
       <c r="Q9" s="29"/>
@@ -2147,32 +2119,32 @@
     </row>
     <row r="10" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C10" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="43">
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P10" s="29"/>
       <c r="Q10" s="29"/>
@@ -2228,36 +2200,36 @@
     </row>
     <row r="11" spans="1:92" x14ac:dyDescent="0.35">
       <c r="C11" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="12">
         <v>3.3570000000000002</v>
       </c>
       <c r="G11" s="12"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="43">
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="41">
         <f t="shared" si="0"/>
         <v>3.3570000000000002</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P11" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q11" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R11" s="15" t="s">
         <v>73</v>
@@ -2318,9 +2290,9 @@
       <c r="E12" s="11"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="43" t="str">
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2367,10 +2339,10 @@
       <c r="AC12" s="27"/>
       <c r="AD12" s="36"/>
       <c r="AE12" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF12" s="36" t="s">
         <v>100</v>
-      </c>
-      <c r="AF12" s="36" t="s">
-        <v>101</v>
       </c>
       <c r="AG12" s="36"/>
       <c r="AH12" s="35"/>
@@ -2394,9 +2366,9 @@
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="43" t="str">
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2472,9 +2444,9 @@
       <c r="E14" s="11"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="43" t="str">
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2591,9 +2563,9 @@
       <c r="E15" s="11"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="43" t="str">
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2713,9 +2685,9 @@
       <c r="E16" s="11"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="43" t="str">
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2835,9 +2807,9 @@
       <c r="E17" s="11"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="43" t="str">
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -2953,9 +2925,9 @@
       <c r="E18" s="11"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="43" t="str">
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3068,9 +3040,9 @@
       <c r="E19" s="11"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="43" t="str">
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="41" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -3181,18 +3153,18 @@
       <c r="CN19" s="2"/>
     </row>
     <row r="20" spans="1:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E20" s="48" t="str">
+      <c r="E20" s="46" t="str">
         <f>CONCATENATE(B2,"_per_",B1)</f>
-        <v>nonprofiled_consumption_per_ga_brp_es</v>
-      </c>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="49" t="s">
+        <v>nonprofiled_consumption_per_ga</v>
+      </c>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="J20" s="50"/>
-      <c r="K20" s="51"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="49"/>
       <c r="R20" s="15" t="s">
         <v>74</v>
       </c>
@@ -3432,11 +3404,11 @@
       <c r="A22" s="2"/>
       <c r="B22" s="16" t="str">
         <f>IF(AND(F22&lt;&gt;"null",F22&lt;&gt;""),IF(F22=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G22&lt;&gt;"null",G22&lt;&gt;""),IF(G22=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E22=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
-        <v/>
+        <v>glmp</v>
       </c>
       <c r="C22" s="16" t="str">
         <f>IF(AND(F22&lt;&gt;"null",F22&lt;&gt;""),IF(F22=INDEX(TableDay1[es_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(AND(G22&lt;&gt;"null",G22&lt;&gt;""),IF(G22=INDEX(TableDay1[brp_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(E22=INDEX(TableDay1[ga_id],MATCH("SKMP",TableDay1[note],0),1),"skmp","")))</f>
-        <v/>
+        <v>skmp</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>72</v>
@@ -3447,11 +3419,11 @@
       </c>
       <c r="F22" s="31" t="str">
         <f>IF(B$1="ga",IF(E22="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$2=0,"",AE$2),IF(B$1="ga_brp",IF(G22="","","null"))))</f>
-        <v>3000000000000</v>
+        <v>null</v>
       </c>
       <c r="G22" s="31" t="str">
         <f>IF(B$1="ga",IF(E22="","","null"),IF(B$1="ga_es",IF(F22="","","null"),IF(B$1="ga_brp",IF(AF$2=0,"",AF$2),IF(F22="","",INDEX(TableDay1[brp_id],MATCH(F22,TableDay1[es_id],0),1)))))</f>
-        <v>3300000000000</v>
+        <v>null</v>
       </c>
       <c r="H22" s="33" t="str">
         <f ca="1">IF(E22="","",SUBSTITUTE(ROUND(I22+J22+K22,3),",","."))</f>
@@ -3574,11 +3546,11 @@
     <row r="23" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B23" s="16" t="str">
         <f>IF(AND(F23&lt;&gt;"null",F23&lt;&gt;""),IF(F23=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G23&lt;&gt;"null",G23&lt;&gt;""),IF(G23=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E23=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
-        <v/>
+        <v>glmp</v>
       </c>
       <c r="C23" s="16" t="str">
         <f>IF(AND(F23&lt;&gt;"null",F23&lt;&gt;""),IF(F23=INDEX(TableDay1[es_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(AND(G23&lt;&gt;"null",G23&lt;&gt;""),IF(G23=INDEX(TableDay1[brp_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(E23=INDEX(TableDay1[ga_id],MATCH("SKMP",TableDay1[note],0),1),"skmp","")))</f>
-        <v/>
+        <v>skmp</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>73</v>
@@ -3589,11 +3561,11 @@
       </c>
       <c r="F23" s="31" t="str">
         <f>IF(B$1="ga",IF(E23="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$2=0,"",AE$2),IF(B$1="ga_brp",IF(G23="","","null"))))</f>
-        <v>3000000000000</v>
+        <v>null</v>
       </c>
       <c r="G23" s="31" t="str">
         <f>IF(B$1="ga",IF(E23="","","null"),IF(B$1="ga_es",IF(F23="","","null"),IF(B$1="ga_brp",IF(AF$2=0,"",AF$2),IF(F23="","",INDEX(TableDay1[brp_id],MATCH(F23,TableDay1[es_id],0),1)))))</f>
-        <v>3300000000000</v>
+        <v>null</v>
       </c>
       <c r="H23" s="33" t="str">
         <f t="shared" ref="H23:H45" ca="1" si="7">IF(E23="","",SUBSTITUTE(ROUND(I23+J23+K23,3),",","."))</f>
@@ -3719,11 +3691,11 @@
     <row r="24" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B24" s="16" t="str">
         <f>IF(AND(F24&lt;&gt;"null",F24&lt;&gt;""),IF(F24=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G24&lt;&gt;"null",G24&lt;&gt;""),IF(G24=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E24=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
-        <v/>
+        <v>glmp</v>
       </c>
       <c r="C24" s="16" t="str">
         <f>IF(AND(F24&lt;&gt;"null",F24&lt;&gt;""),IF(F24=INDEX(TableDay1[es_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(AND(G24&lt;&gt;"null",G24&lt;&gt;""),IF(G24=INDEX(TableDay1[brp_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(E24=INDEX(TableDay1[ga_id],MATCH("SKMP",TableDay1[note],0),1),"skmp","")))</f>
-        <v/>
+        <v>skmp</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>74</v>
@@ -3734,11 +3706,11 @@
       </c>
       <c r="F24" s="31" t="str">
         <f>IF(B$1="ga",IF(E24="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$2=0,"",AE$2),IF(B$1="ga_brp",IF(G24="","","null"))))</f>
-        <v>3000000000000</v>
+        <v>null</v>
       </c>
       <c r="G24" s="31" t="str">
         <f>IF(B$1="ga",IF(E24="","","null"),IF(B$1="ga_es",IF(F24="","","null"),IF(B$1="ga_brp",IF(AF$2=0,"",AF$2),IF(F24="","",INDEX(TableDay1[brp_id],MATCH(F24,TableDay1[es_id],0),1)))))</f>
-        <v>3300000000000</v>
+        <v>null</v>
       </c>
       <c r="H24" s="33" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -3867,11 +3839,11 @@
     <row r="25" spans="1:92" x14ac:dyDescent="0.35">
       <c r="B25" s="16" t="str">
         <f>IF(AND(F25&lt;&gt;"null",F25&lt;&gt;""),IF(F25=INDEX(TableDay1[es_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(AND(G25&lt;&gt;"null",G25&lt;&gt;""),IF(G25=INDEX(TableDay1[brp_id],MATCH("GLMP",TableDay1[note],0),1),"glmp",""),IF(E25=INDEX(TableDay1[ga_id],MATCH("GLMP",TableDay1[note],0),1),"glmp","")))</f>
-        <v/>
+        <v>glmp</v>
       </c>
       <c r="C25" s="16" t="str">
         <f>IF(AND(F25&lt;&gt;"null",F25&lt;&gt;""),IF(F25=INDEX(TableDay1[es_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(AND(G25&lt;&gt;"null",G25&lt;&gt;""),IF(G25=INDEX(TableDay1[brp_id],MATCH("SKMP",TableDay1[note],0),1),"skmp",""),IF(E25=INDEX(TableDay1[ga_id],MATCH("SKMP",TableDay1[note],0),1),"skmp","")))</f>
-        <v/>
+        <v>skmp</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>75</v>
@@ -3882,11 +3854,11 @@
       </c>
       <c r="F25" s="31" t="str">
         <f>IF(B$1="ga",IF(E25="","","null"),IF(OR(B$1="ga_es",B$1="ga_brp_es"),IF(AE$2=0,"",AE$2),IF(B$1="ga_brp",IF(G25="","","null"))))</f>
-        <v>3000000000000</v>
+        <v>null</v>
       </c>
       <c r="G25" s="31" t="str">
         <f>IF(B$1="ga",IF(E25="","","null"),IF(B$1="ga_es",IF(F25="","","null"),IF(B$1="ga_brp",IF(AF$2=0,"",AF$2),IF(F25="","",INDEX(TableDay1[brp_id],MATCH(F25,TableDay1[es_id],0),1)))))</f>
-        <v>3300000000000</v>
+        <v>null</v>
       </c>
       <c r="H25" s="33" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -5343,10 +5315,10 @@
         <f>SUMIFS(TableDay1[TotalHour],TableDay1[settlement_method],"D01",TableDay1[resolution],"PT1H")</f>
         <v>0</v>
       </c>
-      <c r="W35" s="16" t="s">
+      <c r="W35" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="X35" s="16"/>
+      <c r="X35" s="55"/>
       <c r="Y35" s="28">
         <f>SUM(Y37:Y40)</f>
         <v>0</v>
@@ -6134,10 +6106,10 @@
         <f>SUMIFS(TableDay1[TotalHour],TableDay1[type],"E18",TableDay1[resolution],"PT1H")</f>
         <v>40.158999999999999</v>
       </c>
-      <c r="W41" s="39" t="s">
+      <c r="W41" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="X41" s="40"/>
+      <c r="X41" s="55"/>
       <c r="Y41" s="28">
         <f>SUM(Y43:Y46)</f>
         <v>40.158999999999999</v>
@@ -6744,12 +6716,12 @@
     </row>
     <row r="46" spans="1:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C46" s="2"/>
-      <c r="E46" s="48" t="s">
+      <c r="E46" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="48"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="48"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
       <c r="R46" s="24"/>
       <c r="S46" s="24"/>
       <c r="T46" s="24"/>
@@ -6868,10 +6840,10 @@
         <f>SUMIFS(TableDay1[TotalHour],TableDay1[settlement_method],"E02",TableDay1[resolution],"PT1H")</f>
         <v>20</v>
       </c>
-      <c r="W47" s="39" t="s">
+      <c r="W47" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="X47" s="40"/>
+      <c r="X47" s="55"/>
       <c r="Y47" s="28">
         <f>SUM(Y49:Y52)</f>
         <v>20</v>
@@ -7420,12 +7392,12 @@
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-      <c r="E52" s="52" t="s">
+      <c r="E52" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="54"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="51"/>
+      <c r="H52" s="52"/>
       <c r="R52" s="24"/>
       <c r="S52" s="24"/>
       <c r="T52" s="24"/>
@@ -7546,10 +7518,10 @@
         <f>ROUND(SUMIFS(TableDay1[TotalHour],TableDay1[type],"E20",TableDay1[resolution],"PT1H",TableDay1[to_ga],$AD$2),3)</f>
         <v>3.3570000000000002</v>
       </c>
-      <c r="W53" s="39" t="s">
+      <c r="W53" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="X53" s="40"/>
+      <c r="X53" s="55"/>
       <c r="Y53" s="28">
         <f>ROUND(SUM(Y55:Y58),3)</f>
         <v>3.3570000000000002</v>
@@ -7650,8 +7622,8 @@
         <f>SUBSTITUTE(ROUND(H54,3),",",".")</f>
         <v>0</v>
       </c>
-      <c r="Q54" s="46"/>
-      <c r="R54" s="46"/>
+      <c r="Q54" s="44"/>
+      <c r="R54" s="44"/>
       <c r="S54" s="24"/>
       <c r="T54" s="24"/>
       <c r="U54" s="6" t="s">
@@ -7765,7 +7737,7 @@
         <f t="shared" ref="I55:I57" si="16">SUBSTITUTE(ROUND(H55,3),",",".")</f>
         <v>0</v>
       </c>
-      <c r="R55" s="44"/>
+      <c r="R55" s="42"/>
       <c r="S55" s="24"/>
       <c r="T55" s="24"/>
       <c r="U55" s="15" t="s">
@@ -7788,7 +7760,7 @@
         <f>ROUND(V55,3)</f>
         <v>0.83899999999999997</v>
       </c>
-      <c r="AA55" s="45"/>
+      <c r="AA55" s="43"/>
       <c r="AB55" s="2"/>
       <c r="AC55" s="2"/>
       <c r="AD55" s="2"/>
@@ -7906,7 +7878,7 @@
         <f>ROUND(V56,3)</f>
         <v>0.83899999999999997</v>
       </c>
-      <c r="AA56" s="45"/>
+      <c r="AA56" s="43"/>
       <c r="AB56" s="2"/>
       <c r="AC56" s="2"/>
       <c r="AD56" s="2"/>
@@ -8024,7 +7996,7 @@
         <f>ROUND(V57,3)</f>
         <v>0.83899999999999997</v>
       </c>
-      <c r="AA57" s="45"/>
+      <c r="AA57" s="43"/>
       <c r="AB57" s="2"/>
       <c r="AC57" s="2"/>
       <c r="AD57" s="2"/>
@@ -8095,12 +8067,12 @@
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
-      <c r="E58" s="52" t="s">
+      <c r="E58" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="F58" s="53"/>
-      <c r="G58" s="53"/>
-      <c r="H58" s="54"/>
+      <c r="F58" s="51"/>
+      <c r="G58" s="51"/>
+      <c r="H58" s="52"/>
       <c r="R58" s="24"/>
       <c r="S58" s="24"/>
       <c r="T58" s="24"/>
@@ -8127,7 +8099,7 @@
         <f>ROUND(V58,3)</f>
         <v>0.83899999999999997</v>
       </c>
-      <c r="AA58" s="45"/>
+      <c r="AA58" s="43"/>
       <c r="AB58" s="2"/>
       <c r="AC58" s="2"/>
       <c r="AD58" s="2"/>
@@ -8221,10 +8193,10 @@
         <f>ROUND(SUMIFS(TableDay1[TotalHour],TableDay1[type],"E20",TableDay1[resolution],"PT1H",TableDay1[from_ga],"800"),3)</f>
         <v>0</v>
       </c>
-      <c r="W59" s="39" t="s">
+      <c r="W59" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="X59" s="40"/>
+      <c r="X59" s="55"/>
       <c r="Y59" s="28">
         <f>ROUND(SUM(Y61:Y64),3)</f>
         <v>0</v>
@@ -8323,7 +8295,7 @@
         <f>SUBSTITUTE(ROUND(H60,3),",",".")</f>
         <v>10.04</v>
       </c>
-      <c r="R60" s="44"/>
+      <c r="R60" s="42"/>
       <c r="S60" s="24"/>
       <c r="T60" s="24"/>
       <c r="U60" s="6" t="s">
@@ -8458,7 +8430,7 @@
         <f>ROUND(V61,3)</f>
         <v>0</v>
       </c>
-      <c r="AA61" s="45"/>
+      <c r="AA61" s="43"/>
       <c r="AB61" s="2"/>
       <c r="AC61" s="2"/>
       <c r="AD61" s="2"/>
@@ -8574,7 +8546,7 @@
         <f>ROUND(V62,3)</f>
         <v>0</v>
       </c>
-      <c r="AA62" s="45"/>
+      <c r="AA62" s="43"/>
       <c r="AB62" s="2"/>
       <c r="AC62" s="2"/>
       <c r="AD62" s="2"/>
@@ -8690,7 +8662,7 @@
         <f>ROUND(V63,3)</f>
         <v>0</v>
       </c>
-      <c r="AA63" s="45"/>
+      <c r="AA63" s="43"/>
       <c r="AB63" s="2"/>
       <c r="AC63" s="2"/>
       <c r="AD63" s="2"/>
@@ -8759,12 +8731,12 @@
     </row>
     <row r="64" spans="1:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C64" s="2"/>
-      <c r="E64" s="52" t="s">
+      <c r="E64" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="F64" s="53"/>
-      <c r="G64" s="53"/>
-      <c r="H64" s="54"/>
+      <c r="F64" s="51"/>
+      <c r="G64" s="51"/>
+      <c r="H64" s="52"/>
       <c r="R64" s="24"/>
       <c r="S64" s="24"/>
       <c r="T64" s="24"/>
@@ -8791,7 +8763,7 @@
         <f>ROUND(V64,3)</f>
         <v>0</v>
       </c>
-      <c r="AA64" s="45"/>
+      <c r="AA64" s="43"/>
       <c r="AB64" s="2"/>
       <c r="AC64" s="2"/>
       <c r="AD64" s="2"/>
@@ -8883,10 +8855,10 @@
         <f>ROUND(SUMIFS(TableDay1[TotalHour],TableDay1[type],"E17",TableDay1[resolution],"PT1H"),3)</f>
         <v>20</v>
       </c>
-      <c r="W65" s="56" t="s">
+      <c r="W65" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="X65" s="57"/>
+      <c r="X65" s="55"/>
       <c r="Y65" s="28">
         <f>ROUND(SUM(Y67:Y70),3)</f>
         <v>20</v>
@@ -9422,12 +9394,12 @@
     </row>
     <row r="70" spans="3:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C70" s="2"/>
-      <c r="E70" s="52" t="s">
+      <c r="E70" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="F70" s="53"/>
-      <c r="G70" s="53"/>
-      <c r="H70" s="54"/>
+      <c r="F70" s="51"/>
+      <c r="G70" s="51"/>
+      <c r="H70" s="52"/>
       <c r="R70" s="24"/>
       <c r="S70" s="24"/>
       <c r="T70" s="27"/>
@@ -10011,12 +9983,12 @@
     </row>
     <row r="76" spans="3:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C76" s="2"/>
-      <c r="E76" s="52" t="s">
+      <c r="E76" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="F76" s="53"/>
-      <c r="G76" s="53"/>
-      <c r="H76" s="54"/>
+      <c r="F76" s="51"/>
+      <c r="G76" s="51"/>
+      <c r="H76" s="52"/>
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
@@ -10634,12 +10606,12 @@
     </row>
     <row r="82" spans="3:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C82" s="2"/>
-      <c r="E82" s="52" t="s">
+      <c r="E82" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="F82" s="53"/>
-      <c r="G82" s="53"/>
-      <c r="H82" s="54"/>
+      <c r="F82" s="51"/>
+      <c r="G82" s="51"/>
+      <c r="H82" s="52"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
@@ -10852,13 +10824,13 @@
       </c>
       <c r="J84" s="2"/>
       <c r="U84" s="2"/>
-      <c r="V84" s="55" t="s">
+      <c r="V84" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="W84" s="55"/>
-      <c r="X84" s="55"/>
-      <c r="Y84" s="55"/>
-      <c r="Z84" s="55"/>
+      <c r="W84" s="53"/>
+      <c r="X84" s="53"/>
+      <c r="Y84" s="53"/>
+      <c r="Z84" s="53"/>
       <c r="AA84" s="2"/>
       <c r="AB84" s="2"/>
       <c r="AC84" s="2"/>
@@ -11262,13 +11234,13 @@
     </row>
     <row r="88" spans="3:92" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C88" s="2"/>
-      <c r="E88" s="52" t="s">
+      <c r="E88" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="F88" s="53"/>
-      <c r="G88" s="53"/>
-      <c r="H88" s="53"/>
-      <c r="I88" s="54"/>
+      <c r="F88" s="51"/>
+      <c r="G88" s="51"/>
+      <c r="H88" s="51"/>
+      <c r="I88" s="52"/>
       <c r="J88" s="2"/>
       <c r="R88" s="2"/>
       <c r="S88" s="2"/>
@@ -11380,7 +11352,7 @@
         <v>2</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J89" s="2"/>
       <c r="R89" s="2"/>
@@ -40688,7 +40660,9 @@
       <c r="CN400" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="18">
+    <mergeCell ref="W53:X53"/>
+    <mergeCell ref="W59:X59"/>
     <mergeCell ref="AH1:AK1"/>
     <mergeCell ref="E20:H20"/>
     <mergeCell ref="I20:K20"/>
@@ -40702,6 +40676,9 @@
     <mergeCell ref="E76:H76"/>
     <mergeCell ref="E82:H82"/>
     <mergeCell ref="W65:X65"/>
+    <mergeCell ref="W35:X35"/>
+    <mergeCell ref="W41:X41"/>
+    <mergeCell ref="W47:X47"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="F2:I19">
@@ -40770,11 +40747,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="17d0a144-7218-432a-80c1-1473a2ac0f84" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -40954,26 +40932,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="17d0a144-7218-432a-80c1-1473a2ac0f84" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B51BD707-A63C-4C12-A5D3-024A5FAE9E8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4F67E43-074E-4C0F-B170-E53BCA717C8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="17d0a144-7218-432a-80c1-1473a2ac0f84"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -40997,9 +40966,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4F67E43-074E-4C0F-B170-E53BCA717C8F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B51BD707-A63C-4C12-A5D3-024A5FAE9E8F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="17d0a144-7218-432a-80c1-1473a2ac0f84"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>